<commit_message>
PROJECT REQUIREMENTS FOR 3/16/2015 - SECOND ITERATION received Friday, February 20, 2015 5:52 PM
</commit_message>
<xml_diff>
--- a/etc/pm/requirements/Pre-K Finder and Form Modifications 2015 - Round 2.xlsx
+++ b/etc/pm/requirements/Pre-K Finder and Form Modifications 2015 - Round 2.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="48">
   <si>
     <t>Requirement</t>
   </si>
@@ -242,13 +242,327 @@
   </si>
   <si>
     <t>Put a Help "?" icon next to the House Number field.  If the user clicks on that "?" Icon, then a bubble pops up to say "If you live at 52 Chambers Street, the House Number is 52"</t>
+  </si>
+  <si>
+    <t>App</t>
+  </si>
+  <si>
+    <t>Add the "Get in Touch" button (leading to the generic Form) to the District School entries on the List</t>
+  </si>
+  <si>
+    <t>Add the "Get in Touch" button (leading to the generic Form) to the District School bubble  arrived at via the "Map" function</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">"Details" Button.  Currently if a user clicks the details button on the site, the cell shifts down to display the seat capacity for FD and HD seats.   The ask is this now:  When the user clicks the "Details" button in the enhanced App, we would like a new box to flip open to the left of the original site cell to display a good deal of more information about the site.   As this will be new data that the App has not displayed before, we will also have to build this into the Data Integration piece of the data that is send to DoiTT on a regular basis.   </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Please see attached for our mockup of how that should look</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.</t>
+    </r>
+  </si>
+  <si>
+    <t>We would also like that same Details button added to the site bubble arrived at via the "Map" function</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Please see attached </t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">We should elimate all references to </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Calling 311</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> on some sites, although lets keep that space for displaying different information (see below)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>By March 16, we are only going to be displaying sites in the Pre-K Finder open for the 2015-16 school year</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.   For new sites coming on, we would like to use the space vacated by the Calling 311 to have the App display "</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Opening in September 2015</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>".  Data Integration will require that we send to DoITT which sites are new.</t>
+    </r>
+  </si>
+  <si>
+    <t>Add to the banner at the top "(for the 2015-16 School year)" after "Pre-K Finder".  Probably in a different font type and/or size.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Currently the Pre-K Finder only allows a parent to search by Address.  We would like the parent to be allowed to search by Site Name as well. </t>
+  </si>
+  <si>
+    <t>Currently, if you click on a Site in the map, the corresponding sidebar List does not change (assumedly it stays focussed on your current GPS location).  Could the List dynamically refresh to show the sites closest to the Site that the parent has chosen on the map?</t>
+  </si>
+  <si>
+    <t>This is a  "Nice to Have"</t>
+  </si>
+  <si>
+    <t>The followinq requirements are what need to go-live on the morning of March 16th:</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">We need to add a new </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>program type</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> filter called "5-Hour", in addition to the ones already there for "Half Day", "Full Day" and "All".   User should be allowed to filter on 1-2 program type options at a time (e.g. parent wants to look at all 5-Hour </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>and</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Half Day programs).  Data Integration will require that we label each site with the program type(s) that it offers.</t>
+    </r>
+  </si>
+  <si>
+    <t>Add a same "Get in Touch" button to the top navy blue banner of the Pre-K Finder.  Same formatting as on the List except Orange background, White lettering, and highlight hovering.  Positioned at center.   Clicking this button will lead parent to the information Form.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">We need to add a new </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Site type</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> filter called "Charter Schools", in addition to the ones already there for "District Schools", "Early Ed Centers" and "All".   User should be allowed to filter on 1-2 site type options at a time (e.g. parent wants to look at all Charter Schools </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>and</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Early Ed Centers).  Data Integration will require that we label each site with its Site type.</t>
+    </r>
+  </si>
+  <si>
+    <t>On the morning of April 25th, the application period in SEMS has ended.  We should then revert back to the "Get in Touch" button at the top center of the screen and each site cell should revert back to the "Get in Touch" button.   All those Get in Touch buttons lead the parent to the Information Form.</t>
+  </si>
+  <si>
+    <t>On the morning of March 16th, the "Get in Touch" button on the top banner (if it exists yet) should change to read "I still would like more information about Pre-K".   Size of the button might need to increase, and it should shift to slightly left of center.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">On the morning of March 16th, a new button should appear on the top banner, slightly right of center, that should read "I am ready to apply for Pre-K".  When the parent clicks on that button, a </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>new tab</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> should open up in their browser to the following URL:  www.semsnycdoe.com/parentsite </t>
+    </r>
+  </si>
+  <si>
+    <t>On the morning of March 16th, for all District Schools and Early Ed Centers offering Full Day seats, the "Get in Touch" button in their List cell should change to read "Apply Now".  If a parent clicks on that Apply button, a new tab should open up in their browser to the following URL:  www.semsnycdoe.com/parentsite</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">On the morning of March 16th, for all Charter Schools, and for Early Ed Centers offering </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">only </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Half Day or 5-Hour seats, the "Get in Touch" should remain as such and still point to the Information Form.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">On the morning of March 16th, in the upper right corner of the top banner, to the left of the Map/List button, we would like a link to display “View the Pre-K Directory for More Info” and if a user clicks on that link a </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>new tab</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> opens in their broswer  to the following URL: http://schools.nyc.gov/ChoicesEnrollment/PreK/Resources/default.htm </t>
+    </r>
+  </si>
+  <si>
+    <t>Tentative - final answer on Monday</t>
+  </si>
+  <si>
+    <t>Ideally requirements 12-14 could get implemented ahead of March 16</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -293,13 +607,27 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFC00000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -314,7 +642,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -334,11 +662,26 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -641,7 +984,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F12"/>
+  <dimension ref="A1:F33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -655,7 +998,7 @@
     <col min="3" max="3" width="82.85546875" style="4" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="8.5703125" style="3" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9.42578125" style="3" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="22.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="64.140625" style="3" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="11.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -736,7 +1079,7 @@
         <v>23</v>
       </c>
       <c r="E6" s="5"/>
-      <c r="F6" s="7" t="s">
+      <c r="F6" s="13" t="s">
         <v>22</v>
       </c>
     </row>
@@ -761,7 +1104,7 @@
       <c r="C8" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="F8" s="8" t="s">
+      <c r="F8" s="12" t="s">
         <v>20</v>
       </c>
     </row>
@@ -775,7 +1118,7 @@
       <c r="C9" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="F9" s="8"/>
+      <c r="F9" s="12"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
@@ -787,7 +1130,7 @@
       <c r="C10" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="F10" s="8"/>
+      <c r="F10" s="12"/>
     </row>
     <row r="11" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="3">
@@ -809,6 +1152,229 @@
       </c>
       <c r="C12" s="4" t="s">
         <v>18</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A13" s="3">
+        <v>12</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="D13"/>
+      <c r="E13"/>
+      <c r="F13" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A14" s="3">
+        <v>13</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="D14"/>
+      <c r="E14"/>
+      <c r="F14"/>
+    </row>
+    <row r="15" spans="1:6" ht="51" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="3">
+        <v>14</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+      <c r="A16" s="3">
+        <v>15</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+      <c r="A17" s="8">
+        <v>16</v>
+      </c>
+      <c r="B17" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="C17" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="F17" s="10" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="109.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="3">
+        <v>17</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="F18" s="11" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="3">
+        <v>18</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="3">
+        <v>19</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="72" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="3">
+        <v>20</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="3">
+        <v>21</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="3">
+        <v>22</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="56.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="3">
+        <v>23</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="F24" s="3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C26" s="7" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" ht="69.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="3">
+        <v>24</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C28" s="4" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" ht="70.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="3">
+        <v>25</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C29" s="4" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" ht="75.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="3">
+        <v>26</v>
+      </c>
+      <c r="B30" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C30" s="4" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" ht="58.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="8">
+        <v>27</v>
+      </c>
+      <c r="B31" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="C31" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="F31" s="10" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" ht="70.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="3">
+        <v>28</v>
+      </c>
+      <c r="B32" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C32" s="4" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="3">
+        <v>29</v>
+      </c>
+      <c r="B33" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C33" s="4" t="s">
+        <v>40</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
PROJECT REQUIREMENTS FOR 3/16/2015 - SECOND ITERATION received Tuesday, February 24, 2015 3:35 PM
</commit_message>
<xml_diff>
--- a/etc/pm/requirements/Pre-K Finder and Form Modifications 2015 - Round 2.xlsx
+++ b/etc/pm/requirements/Pre-K Finder and Form Modifications 2015 - Round 2.xlsx
@@ -2,24 +2,28 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
-  <workbookPr defaultThemeVersion="124226"/>
+  <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="120" windowWidth="18195" windowHeight="12330"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25605" windowHeight="14235"/>
   </bookViews>
   <sheets>
     <sheet name="Requirements" sheetId="1" r:id="rId1"/>
     <sheet name="Questions" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet1" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Requirements!$A$1:$F$11</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Requirements!$A$1:$G$11</definedName>
   </definedNames>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="70">
   <si>
     <t>Requirement</t>
   </si>
@@ -556,13 +560,79 @@
   </si>
   <si>
     <t>Ideally requirements 12-14 could get implemented ahead of March 16</t>
+  </si>
+  <si>
+    <t>It can be resorted by distance from currently selected site, but this may not be inuitive. How about scroll to current site?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Not really sufficient time to get these out by 3/16 with proper testing on all devices - especially since many of the requested changes cannot be made to meet all devices as identified in these comments </t>
+  </si>
+  <si>
+    <t xml:space="preserve">how many buttons are going in the banner now? Also, new tabs don’t work in iOS standalone mode that is why we have all of the problems with the form in an iframe.  If user creates a desktop shortcut to finder app in iOS and clicks a link or button that opens in a new tab they cannot get back to the finder app without going back to desktop and starting over. </t>
+  </si>
+  <si>
+    <t>see comment on 26</t>
+  </si>
+  <si>
+    <t>what are the dev and stg urls? is there a rule that can applied to this requirement that avoids the need for a code change next year?  (i.e. between certain dates the button has one label vs another) - will this date be the same every year?  Is there a rule that can be applied (i.e. btwn 3nd Monday of march and 4th fri in april)</t>
+  </si>
+  <si>
+    <t>nothing in data currently maps to 5hr prog.  Need to at least know what the value of the day_length field for 5hr will be</t>
+  </si>
+  <si>
+    <t>The app is a single web page that serves all devices.  This requirement will be difficult on mobile due to space limitations. Another option would be to replace the summary content in the list or popup with the detail info and a bacck button or close button.  not all data elements are available in the current data set. is this for the public or internal use?</t>
+  </si>
+  <si>
+    <t>GIS Notes and Questions</t>
+  </si>
+  <si>
+    <t>nothing in data currently maps to charter school.  Need to at least know what the value of the prek_type field for charter school will be… also will this new school type have a different color icon?</t>
+  </si>
+  <si>
+    <t>only district school popup or all schools?</t>
+  </si>
+  <si>
+    <t>The app is a single web page that serves all devices.  This requirement will be difficult on mobile due to space limitations.   Maybe a landing page and a button under the map controls that redisplays landing page?</t>
+  </si>
+  <si>
+    <t>see comments on 18</t>
+  </si>
+  <si>
+    <t>this was orginally a last minute hack fix for last year that aaded this text to the scool name.  The schema should be modified to include a special message field and the code modified to display the message if present.  Data would be provided according to new schema</t>
+  </si>
+  <si>
+    <t>see comments on 19</t>
+  </si>
+  <si>
+    <t>is this for the public or internal use?  Would require a button to toggle btwn search types - see http://maps.nyc.gov/crime</t>
+  </si>
+  <si>
+    <t>see comments on 14</t>
+  </si>
+  <si>
+    <t>It is far better for consistency and accuracy to have separate. If not, it requires working out a design that functions on all devices</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Requires working out a design that functions on all devices - not likely to be room for icon - how about placeholder values to illustrate. </t>
+  </si>
+  <si>
+    <t>Seems unnessary since the only field NOT required now is apt - realestate issue on mobile</t>
+  </si>
+  <si>
+    <t>What is the rule specifically?  Only DOB after what and before what?  How does this rule apply in any given year?</t>
+  </si>
+  <si>
+    <t>Need all desired validation rules not just examples. Example: phone number limited to (###) ###-####, list all other validation rules.</t>
+  </si>
+  <si>
+    <t>Without the ability to select a preferred program, what is the point of the map? As a parent I would find it frustrating to go through the process of selection only to have to provide it later verbally. Seems a simple message "This is NOT an application" may suffice if that is the fear.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -615,6 +685,22 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -639,10 +725,28 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -677,14 +781,35 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="19">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -984,25 +1109,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F33"/>
+  <dimension ref="A1:G36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <pane ySplit="1" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="5" style="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="8.42578125" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="82.85546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.5703125" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.42578125" style="3" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="64.140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="67.28515625" style="4" customWidth="1"/>
+    <col min="4" max="4" width="46.28515625" style="13" customWidth="1"/>
+    <col min="5" max="5" width="8.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="64.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -1012,17 +1138,20 @@
       <c r="C1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" ht="90" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
         <v>1</v>
       </c>
@@ -1032,8 +1161,11 @@
       <c r="C2" s="4" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="D2" s="13" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <v>2</v>
       </c>
@@ -1044,7 +1176,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
         <v>3</v>
       </c>
@@ -1055,7 +1187,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
         <v>4</v>
       </c>
@@ -1065,10 +1197,13 @@
       <c r="C5" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="E5" s="5"/>
+      <c r="D5" s="13" t="s">
+        <v>64</v>
+      </c>
       <c r="F5" s="5"/>
-    </row>
-    <row r="6" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="G5" s="5"/>
+    </row>
+    <row r="6" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
         <v>5</v>
       </c>
@@ -1078,12 +1213,15 @@
       <c r="C6" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="E6" s="5"/>
-      <c r="F6" s="13" t="s">
+      <c r="D6" s="13" t="s">
+        <v>65</v>
+      </c>
+      <c r="F6" s="5"/>
+      <c r="G6" s="12" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
         <v>6</v>
       </c>
@@ -1093,8 +1231,11 @@
       <c r="C7" s="4" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D7" s="13" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="90" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
         <v>7</v>
       </c>
@@ -1104,11 +1245,14 @@
       <c r="C8" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="F8" s="12" t="s">
+      <c r="D8" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="G8" s="14" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
         <v>8</v>
       </c>
@@ -1118,9 +1262,12 @@
       <c r="C9" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="F9" s="12"/>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D9" s="13" t="s">
+        <v>67</v>
+      </c>
+      <c r="G9" s="14"/>
+    </row>
+    <row r="10" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
         <v>9</v>
       </c>
@@ -1130,9 +1277,9 @@
       <c r="C10" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="F10" s="12"/>
-    </row>
-    <row r="11" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="G10" s="14"/>
+    </row>
+    <row r="11" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="3">
         <v>10</v>
       </c>
@@ -1143,7 +1290,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A12" s="3">
         <v>11</v>
       </c>
@@ -1154,7 +1301,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="3">
         <v>12</v>
       </c>
@@ -1164,13 +1311,13 @@
       <c r="C13" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="D13"/>
       <c r="E13"/>
-      <c r="F13" t="s">
+      <c r="F13"/>
+      <c r="G13" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="3">
         <v>13</v>
       </c>
@@ -1180,11 +1327,14 @@
       <c r="C14" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="D14"/>
+      <c r="D14" s="13" t="s">
+        <v>57</v>
+      </c>
       <c r="E14"/>
       <c r="F14"/>
-    </row>
-    <row r="15" spans="1:6" ht="51" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G14"/>
+    </row>
+    <row r="15" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A15" s="3">
         <v>14</v>
       </c>
@@ -1194,8 +1344,11 @@
       <c r="C15" s="4" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+      <c r="D15" s="13" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A16" s="3">
         <v>15</v>
       </c>
@@ -1205,8 +1358,11 @@
       <c r="C16" s="4" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+      <c r="D16" s="13" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="90" x14ac:dyDescent="0.25">
       <c r="A17" s="8">
         <v>16</v>
       </c>
@@ -1216,11 +1372,14 @@
       <c r="C17" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="F17" s="10" t="s">
+      <c r="D17" s="13" t="s">
+        <v>56</v>
+      </c>
+      <c r="G17" s="10" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="109.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" ht="135" x14ac:dyDescent="0.25">
       <c r="A18" s="3">
         <v>17</v>
       </c>
@@ -1230,11 +1389,14 @@
       <c r="C18" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="F18" s="11" t="s">
+      <c r="D18" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="G18" s="11" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" s="3">
         <v>18</v>
       </c>
@@ -1244,8 +1406,11 @@
       <c r="C19" s="4" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="20" spans="1:6" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D19" s="13" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="90" x14ac:dyDescent="0.25">
       <c r="A20" s="3">
         <v>19</v>
       </c>
@@ -1255,8 +1420,11 @@
       <c r="C20" s="4" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="21" spans="1:6" ht="72" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D20" s="13" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A21" s="3">
         <v>20</v>
       </c>
@@ -1266,8 +1434,11 @@
       <c r="C21" s="4" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="22" spans="1:6" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D21" s="13" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A22" s="3">
         <v>21</v>
       </c>
@@ -1278,7 +1449,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="23" spans="1:6" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A23" s="3">
         <v>22</v>
       </c>
@@ -1288,8 +1459,11 @@
       <c r="C23" s="4" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="24" spans="1:6" ht="56.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D23" s="13" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A24" s="3">
         <v>23</v>
       </c>
@@ -1299,16 +1473,22 @@
       <c r="C24" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="F24" s="3" t="s">
+      <c r="D24" s="13" t="s">
+        <v>48</v>
+      </c>
+      <c r="G24" s="3" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="26" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="C26" s="7" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="28" spans="1:6" ht="69.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D26" s="13" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A28" s="3">
         <v>24</v>
       </c>
@@ -1318,8 +1498,11 @@
       <c r="C28" s="4" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="29" spans="1:6" ht="70.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D28" s="13" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A29" s="3">
         <v>25</v>
       </c>
@@ -1329,8 +1512,11 @@
       <c r="C29" s="4" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="30" spans="1:6" ht="75.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D29" s="13" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" ht="105" x14ac:dyDescent="0.25">
       <c r="A30" s="3">
         <v>26</v>
       </c>
@@ -1340,8 +1526,11 @@
       <c r="C30" s="4" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="31" spans="1:6" ht="58.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D30" s="13" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A31" s="8">
         <v>27</v>
       </c>
@@ -1351,11 +1540,14 @@
       <c r="C31" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="F31" s="10" t="s">
+      <c r="D31" s="13" t="s">
+        <v>51</v>
+      </c>
+      <c r="G31" s="10" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="32" spans="1:6" ht="70.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" ht="120" x14ac:dyDescent="0.25">
       <c r="A32" s="3">
         <v>28</v>
       </c>
@@ -1365,8 +1557,11 @@
       <c r="C32" s="4" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="33" spans="1:3" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D32" s="13" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A33" s="3">
         <v>29</v>
       </c>
@@ -1376,14 +1571,30 @@
       <c r="C33" s="4" t="s">
         <v>40</v>
       </c>
+      <c r="D33" s="13" t="s">
+        <v>51</v>
+      </c>
+      <c r="E33"/>
+      <c r="F33"/>
+      <c r="G33"/>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E36"/>
+      <c r="F36"/>
+      <c r="G36"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:F11"/>
+  <autoFilter ref="A1:G11"/>
   <mergeCells count="1">
-    <mergeCell ref="F8:F10"/>
+    <mergeCell ref="G8:G10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -1395,7 +1606,7 @@
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="30.85546875" customWidth="1"/>
   </cols>
@@ -1426,17 +1637,10 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
PROJECT REQUIREMENTS FOR 3/16/2015 - FIRST ITERATION received Wednesday, February 25, 2015 4:38 PM
</commit_message>
<xml_diff>
--- a/etc/pm/requirements/Pre-K Finder and Form Modifications 2015 - Round 2.xlsx
+++ b/etc/pm/requirements/Pre-K Finder and Form Modifications 2015 - Round 2.xlsx
@@ -4,14 +4,14 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25605" windowHeight="14235"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24120" windowHeight="13620"/>
   </bookViews>
   <sheets>
     <sheet name="Requirements" sheetId="1" r:id="rId1"/>
     <sheet name="Questions" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Requirements!$A$1:$G$11</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Requirements!$A$1:$H$11</definedName>
   </definedNames>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="88">
   <si>
     <t>Requirement</t>
   </si>
@@ -556,9 +556,6 @@
     </r>
   </si>
   <si>
-    <t>Tentative - final answer on Monday</t>
-  </si>
-  <si>
     <t>Ideally requirements 12-14 could get implemented ahead of March 16</t>
   </si>
   <si>
@@ -626,13 +623,93 @@
   </si>
   <si>
     <t>Without the ability to select a preferred program, what is the point of the map? As a parent I would find it frustrating to go through the process of selection only to have to provide it later verbally. Seems a simple message "This is NOT an application" may suffice if that is the fear.</t>
+  </si>
+  <si>
+    <t>Map lets you see sites near to a given location (e.g. home, work).  Still has value even if you are not sending a message to a particular program.  This is a business decision that was escalated up.</t>
+  </si>
+  <si>
+    <t>Can shortening the House Number field be done at least?  I willing to strip down the requirement to that.</t>
+  </si>
+  <si>
+    <t>ok - lets go with the placeholder idea</t>
+  </si>
+  <si>
+    <t>ok - but please make sure that user cannot get to the submission confirmation page unless they have filled in all those required fields.  The Red text should come up pointing out why we are not letting them submit the form yet.</t>
+  </si>
+  <si>
+    <t>Phone numbers: ########## (10 numbers)</t>
+  </si>
+  <si>
+    <t>For DOB, I'm willing to say any valid mm/dd/yyyy date from 01/01/2010 up to 12/31/2015</t>
+  </si>
+  <si>
+    <t>all sites should have this.  Only Early Ed Centers currently do.</t>
+  </si>
+  <si>
+    <t>yes we will be adding that to the data and provide that information</t>
+  </si>
+  <si>
+    <t>We would need to see what you mean here.  The current mobile does use a lot of space just for the map/list icons and the "Pre-K Finder text"</t>
+  </si>
+  <si>
+    <t>yes we will be adding that to the data and provide that information.  I suppose new color would be green in keeping in line with DOE colors</t>
+  </si>
+  <si>
+    <t>Data is public use.  Yes we need to provide that data still.  We would need to see what you mean here with your other option proposed.  Possibly when user hits details, the shift down function would just extend additional rows beyond the current one row for seat availability?</t>
+  </si>
+  <si>
+    <t>which comments on 18?</t>
+  </si>
+  <si>
+    <t>ok</t>
+  </si>
+  <si>
+    <t>public use.  Yes something like the crime site, to be able to search by address or site name</t>
+  </si>
+  <si>
+    <t>not sure what this scrolling would look like.  Again, we list this a "nice to have"</t>
+  </si>
+  <si>
+    <t>having this in place by 3/16 is not optional</t>
+  </si>
+  <si>
+    <t>there are none right now.  We are proposing 3 buttons in the banner during the Application period.  This one, plus the "I still need more info about Pre-K", and the "I'm ready to apply for Pre-K".  It sounds like for the mobile devices, the main issue is just real estate on the banner?</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Dates will likely be somewhat different every year.  I'm not aware of a </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>rule</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> we could put in place right now for future years.  There will every year be a start date and and end date, which we communicate well in advance though.  I do not know the dev and stg urls.</t>
+    </r>
+  </si>
+  <si>
+    <t>DP et al. responses</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -701,6 +778,21 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFC00000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FFC00000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -711,7 +803,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -746,7 +838,7 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -769,15 +861,6 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -790,6 +873,25 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="19">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -1109,11 +1211,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G36"/>
+  <dimension ref="A1:H36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D25" sqref="D25"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1121,14 +1223,15 @@
     <col min="1" max="1" width="5" style="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="8.42578125" style="3" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="67.28515625" style="4" customWidth="1"/>
-    <col min="4" max="4" width="46.28515625" style="13" customWidth="1"/>
-    <col min="5" max="5" width="8.42578125" style="3" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.42578125" style="3" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="64.140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="46.28515625" style="10" customWidth="1"/>
+    <col min="5" max="5" width="46.28515625" style="12" customWidth="1"/>
+    <col min="6" max="6" width="8.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="64.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -1139,19 +1242,22 @@
         <v>0</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="E1" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="90" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" ht="90" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
         <v>1</v>
       </c>
@@ -1161,11 +1267,14 @@
       <c r="C2" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="D2" s="13" t="s">
+      <c r="D2" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="E2" s="12" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <v>2</v>
       </c>
@@ -1176,7 +1285,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
         <v>3</v>
       </c>
@@ -1187,7 +1296,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
         <v>4</v>
       </c>
@@ -1197,13 +1306,16 @@
       <c r="C5" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="D5" s="13" t="s">
-        <v>64</v>
-      </c>
-      <c r="F5" s="5"/>
+      <c r="D5" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="E5" s="12" t="s">
+        <v>70</v>
+      </c>
       <c r="G5" s="5"/>
-    </row>
-    <row r="6" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="H5" s="5"/>
+    </row>
+    <row r="6" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
         <v>5</v>
       </c>
@@ -1213,15 +1325,18 @@
       <c r="C6" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="D6" s="13" t="s">
-        <v>65</v>
-      </c>
-      <c r="F6" s="5"/>
-      <c r="G6" s="12" t="s">
+      <c r="D6" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="E6" s="12" t="s">
+        <v>71</v>
+      </c>
+      <c r="G6" s="5"/>
+      <c r="H6" s="9" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
         <v>6</v>
       </c>
@@ -1231,11 +1346,14 @@
       <c r="C7" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="D7" s="13" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" ht="90" x14ac:dyDescent="0.25">
+      <c r="D7" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="E7" s="12" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="90" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
         <v>7</v>
       </c>
@@ -1245,14 +1363,17 @@
       <c r="C8" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="D8" s="13" t="s">
-        <v>68</v>
-      </c>
-      <c r="G8" s="14" t="s">
+      <c r="D8" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="E8" s="12" t="s">
+        <v>73</v>
+      </c>
+      <c r="H8" s="11" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
         <v>8</v>
       </c>
@@ -1262,12 +1383,15 @@
       <c r="C9" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="D9" s="13" t="s">
-        <v>67</v>
-      </c>
-      <c r="G9" s="14"/>
-    </row>
-    <row r="10" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="D9" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="E9" s="12" t="s">
+        <v>74</v>
+      </c>
+      <c r="H9" s="11"/>
+    </row>
+    <row r="10" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
         <v>9</v>
       </c>
@@ -1277,9 +1401,9 @@
       <c r="C10" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="G10" s="14"/>
-    </row>
-    <row r="11" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="H10" s="11"/>
+    </row>
+    <row r="11" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="3">
         <v>10</v>
       </c>
@@ -1290,7 +1414,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="A12" s="3">
         <v>11</v>
       </c>
@@ -1301,7 +1425,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="3">
         <v>12</v>
       </c>
@@ -1311,13 +1435,13 @@
       <c r="C13" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="E13"/>
       <c r="F13"/>
-      <c r="G13" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="G13"/>
+      <c r="H13" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="3">
         <v>13</v>
       </c>
@@ -1327,14 +1451,17 @@
       <c r="C14" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="D14" s="13" t="s">
-        <v>57</v>
-      </c>
-      <c r="E14"/>
+      <c r="D14" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="E14" s="12" t="s">
+        <v>75</v>
+      </c>
       <c r="F14"/>
       <c r="G14"/>
-    </row>
-    <row r="15" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="H14"/>
+    </row>
+    <row r="15" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="A15" s="3">
         <v>14</v>
       </c>
@@ -1344,11 +1471,14 @@
       <c r="C15" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="D15" s="13" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="D15" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="E15" s="12" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="A16" s="3">
         <v>15</v>
       </c>
@@ -1358,28 +1488,34 @@
       <c r="C16" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="D16" s="13" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" ht="90" x14ac:dyDescent="0.25">
-      <c r="A17" s="8">
+      <c r="D16" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="E16" s="12" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" s="18" customFormat="1" ht="90" x14ac:dyDescent="0.25">
+      <c r="A17" s="13">
         <v>16</v>
       </c>
-      <c r="B17" s="8" t="s">
+      <c r="B17" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="C17" s="9" t="s">
+      <c r="C17" s="14" t="s">
         <v>39</v>
       </c>
-      <c r="D17" s="13" t="s">
-        <v>56</v>
-      </c>
-      <c r="G17" s="10" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" ht="135" x14ac:dyDescent="0.25">
+      <c r="D17" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="E17" s="16" t="s">
+        <v>78</v>
+      </c>
+      <c r="F17" s="13"/>
+      <c r="G17" s="13"/>
+      <c r="H17" s="17"/>
+    </row>
+    <row r="18" spans="1:8" ht="135" x14ac:dyDescent="0.25">
       <c r="A18" s="3">
         <v>17</v>
       </c>
@@ -1389,14 +1525,17 @@
       <c r="C18" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="D18" s="13" t="s">
-        <v>54</v>
-      </c>
-      <c r="G18" s="11" t="s">
+      <c r="D18" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="E18" s="12" t="s">
+        <v>79</v>
+      </c>
+      <c r="H18" s="8" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" s="3">
         <v>18</v>
       </c>
@@ -1406,11 +1545,14 @@
       <c r="C19" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="D19" s="13" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" ht="90" x14ac:dyDescent="0.25">
+      <c r="D19" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="E19" s="12" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" ht="90" x14ac:dyDescent="0.25">
       <c r="A20" s="3">
         <v>19</v>
       </c>
@@ -1420,11 +1562,14 @@
       <c r="C20" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="D20" s="13" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="D20" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="E20" s="12" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="A21" s="3">
         <v>20</v>
       </c>
@@ -1434,11 +1579,14 @@
       <c r="C21" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="D21" s="13" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="D21" s="10" t="s">
+        <v>60</v>
+      </c>
+      <c r="E21" s="12" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A22" s="3">
         <v>21</v>
       </c>
@@ -1449,7 +1597,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="23" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A23" s="3">
         <v>22</v>
       </c>
@@ -1459,11 +1607,14 @@
       <c r="C23" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="D23" s="13" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="D23" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="E23" s="12" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A24" s="3">
         <v>23</v>
       </c>
@@ -1473,22 +1624,28 @@
       <c r="C24" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="D24" s="13" t="s">
-        <v>48</v>
-      </c>
-      <c r="G24" s="3" t="s">
+      <c r="D24" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="E24" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="H24" s="3" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="26" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="C26" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="D26" s="13" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="D26" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="E26" s="12" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A28" s="3">
         <v>24</v>
       </c>
@@ -1498,11 +1655,11 @@
       <c r="C28" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="D28" s="13" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="D28" s="10" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="A29" s="3">
         <v>25</v>
       </c>
@@ -1512,11 +1669,11 @@
       <c r="C29" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="D29" s="13" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" ht="105" x14ac:dyDescent="0.25">
+      <c r="D29" s="10" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" ht="105" x14ac:dyDescent="0.25">
       <c r="A30" s="3">
         <v>26</v>
       </c>
@@ -1526,28 +1683,32 @@
       <c r="C30" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="D30" s="13" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A31" s="8">
+      <c r="D30" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="E30" s="12" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" s="18" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A31" s="13">
         <v>27</v>
       </c>
-      <c r="B31" s="8" t="s">
+      <c r="B31" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="C31" s="9" t="s">
+      <c r="C31" s="14" t="s">
         <v>44</v>
       </c>
-      <c r="D31" s="13" t="s">
-        <v>51</v>
-      </c>
-      <c r="G31" s="10" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" ht="120" x14ac:dyDescent="0.25">
+      <c r="D31" s="15" t="s">
+        <v>50</v>
+      </c>
+      <c r="E31" s="16"/>
+      <c r="F31" s="13"/>
+      <c r="G31" s="13"/>
+      <c r="H31" s="17"/>
+    </row>
+    <row r="32" spans="1:8" ht="120" x14ac:dyDescent="0.25">
       <c r="A32" s="3">
         <v>28</v>
       </c>
@@ -1557,11 +1718,14 @@
       <c r="C32" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="D32" s="13" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="D32" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="E32" s="12" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="A33" s="3">
         <v>29</v>
       </c>
@@ -1571,25 +1735,25 @@
       <c r="C33" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="D33" s="13" t="s">
-        <v>51</v>
-      </c>
-      <c r="E33"/>
+      <c r="D33" s="10" t="s">
+        <v>50</v>
+      </c>
       <c r="F33"/>
       <c r="G33"/>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="E36"/>
+      <c r="H33"/>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="F36"/>
       <c r="G36"/>
+      <c r="H36"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:G11"/>
+  <autoFilter ref="A1:H11"/>
   <mergeCells count="1">
-    <mergeCell ref="G8:G10"/>
+    <mergeCell ref="H8:H10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
PROJECT REQUIREMENTS FOR 3/16/2015 - THIRD ITERATION received Wednesday, February 25, 2015 4:38 PM
previous commit message was improperly labeled FIRST ITERATION
</commit_message>
<xml_diff>
--- a/etc/pm/requirements/Pre-K Finder and Form Modifications 2015 - Round 2.xlsx
+++ b/etc/pm/requirements/Pre-K Finder and Form Modifications 2015 - Round 2.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
-  <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25203"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24120" windowHeight="13620"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24120" windowHeight="13620" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Requirements" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="89">
   <si>
     <t>Requirement</t>
   </si>
@@ -703,6 +703,9 @@
   </si>
   <si>
     <t>DP et al. responses</t>
+  </si>
+  <si>
+    <t>x</t>
   </si>
 </sst>
 </file>
@@ -870,9 +873,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -892,6 +892,9 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="19">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -1213,25 +1216,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="5" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.42578125" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="67.28515625" style="4" customWidth="1"/>
-    <col min="4" max="4" width="46.28515625" style="10" customWidth="1"/>
-    <col min="5" max="5" width="46.28515625" style="12" customWidth="1"/>
-    <col min="6" max="6" width="8.42578125" style="3" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.42578125" style="3" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="64.140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.5" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="67.33203125" style="4" customWidth="1"/>
+    <col min="4" max="4" width="46.33203125" style="10" customWidth="1"/>
+    <col min="5" max="5" width="46.33203125" style="11" customWidth="1"/>
+    <col min="6" max="6" width="8.5" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.5" style="3" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="64.1640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -1257,7 +1260,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="90" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" ht="70">
       <c r="A2" s="3">
         <v>1</v>
       </c>
@@ -1270,11 +1273,11 @@
       <c r="D2" s="10" t="s">
         <v>68</v>
       </c>
-      <c r="E2" s="12" t="s">
+      <c r="E2" s="11" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" ht="42">
       <c r="A3" s="3">
         <v>2</v>
       </c>
@@ -1285,7 +1288,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8">
       <c r="A4" s="3">
         <v>3</v>
       </c>
@@ -1296,7 +1299,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" ht="56">
       <c r="A5" s="3">
         <v>4</v>
       </c>
@@ -1309,13 +1312,13 @@
       <c r="D5" s="10" t="s">
         <v>63</v>
       </c>
-      <c r="E5" s="12" t="s">
+      <c r="E5" s="11" t="s">
         <v>70</v>
       </c>
       <c r="G5" s="5"/>
       <c r="H5" s="5"/>
     </row>
-    <row r="6" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" ht="42">
       <c r="A6" s="3">
         <v>5</v>
       </c>
@@ -1328,7 +1331,7 @@
       <c r="D6" s="10" t="s">
         <v>64</v>
       </c>
-      <c r="E6" s="12" t="s">
+      <c r="E6" s="11" t="s">
         <v>71</v>
       </c>
       <c r="G6" s="5"/>
@@ -1336,7 +1339,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" ht="56">
       <c r="A7" s="3">
         <v>6</v>
       </c>
@@ -1349,11 +1352,11 @@
       <c r="D7" s="10" t="s">
         <v>65</v>
       </c>
-      <c r="E7" s="12" t="s">
+      <c r="E7" s="11" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="90" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" ht="70">
       <c r="A8" s="3">
         <v>7</v>
       </c>
@@ -1366,14 +1369,14 @@
       <c r="D8" s="10" t="s">
         <v>67</v>
       </c>
-      <c r="E8" s="12" t="s">
+      <c r="E8" s="11" t="s">
         <v>73</v>
       </c>
-      <c r="H8" s="11" t="s">
+      <c r="H8" s="18" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" ht="28">
       <c r="A9" s="3">
         <v>8</v>
       </c>
@@ -1386,12 +1389,12 @@
       <c r="D9" s="10" t="s">
         <v>66</v>
       </c>
-      <c r="E9" s="12" t="s">
+      <c r="E9" s="11" t="s">
         <v>74</v>
       </c>
-      <c r="H9" s="11"/>
-    </row>
-    <row r="10" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="H9" s="18"/>
+    </row>
+    <row r="10" spans="1:8">
       <c r="A10" s="3">
         <v>9</v>
       </c>
@@ -1401,9 +1404,9 @@
       <c r="C10" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="H10" s="11"/>
-    </row>
-    <row r="11" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="H10" s="18"/>
+    </row>
+    <row r="11" spans="1:8" ht="28">
       <c r="A11" s="3">
         <v>10</v>
       </c>
@@ -1414,7 +1417,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" ht="56">
       <c r="A12" s="3">
         <v>11</v>
       </c>
@@ -1425,7 +1428,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" ht="28">
       <c r="A13" s="3">
         <v>12</v>
       </c>
@@ -1441,7 +1444,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" ht="28">
       <c r="A14" s="3">
         <v>13</v>
       </c>
@@ -1454,14 +1457,14 @@
       <c r="D14" s="10" t="s">
         <v>56</v>
       </c>
-      <c r="E14" s="12" t="s">
+      <c r="E14" s="11" t="s">
         <v>75</v>
       </c>
       <c r="F14"/>
       <c r="G14"/>
       <c r="H14"/>
     </row>
-    <row r="15" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" ht="56">
       <c r="A15" s="3">
         <v>14</v>
       </c>
@@ -1474,11 +1477,11 @@
       <c r="D15" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="E15" s="12" t="s">
+      <c r="E15" s="11" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="16" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" ht="70">
       <c r="A16" s="3">
         <v>15</v>
       </c>
@@ -1491,31 +1494,31 @@
       <c r="D16" s="10" t="s">
         <v>52</v>
       </c>
-      <c r="E16" s="12" t="s">
+      <c r="E16" s="11" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="17" spans="1:8" s="18" customFormat="1" ht="90" x14ac:dyDescent="0.25">
-      <c r="A17" s="13">
+    <row r="17" spans="1:8" s="17" customFormat="1" ht="70">
+      <c r="A17" s="12">
         <v>16</v>
       </c>
-      <c r="B17" s="13" t="s">
+      <c r="B17" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="C17" s="14" t="s">
+      <c r="C17" s="13" t="s">
         <v>39</v>
       </c>
-      <c r="D17" s="15" t="s">
+      <c r="D17" s="14" t="s">
         <v>55</v>
       </c>
-      <c r="E17" s="16" t="s">
+      <c r="E17" s="15" t="s">
         <v>78</v>
       </c>
-      <c r="F17" s="13"/>
-      <c r="G17" s="13"/>
-      <c r="H17" s="17"/>
-    </row>
-    <row r="18" spans="1:8" ht="135" x14ac:dyDescent="0.25">
+      <c r="F17" s="12"/>
+      <c r="G17" s="12"/>
+      <c r="H17" s="16"/>
+    </row>
+    <row r="18" spans="1:8" ht="98">
       <c r="A18" s="3">
         <v>17</v>
       </c>
@@ -1528,14 +1531,14 @@
       <c r="D18" s="10" t="s">
         <v>53</v>
       </c>
-      <c r="E18" s="12" t="s">
+      <c r="E18" s="11" t="s">
         <v>79</v>
       </c>
       <c r="H18" s="8" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="19" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" ht="28">
       <c r="A19" s="3">
         <v>18</v>
       </c>
@@ -1548,11 +1551,11 @@
       <c r="D19" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="E19" s="12" t="s">
+      <c r="E19" s="11" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="20" spans="1:8" ht="90" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" ht="70">
       <c r="A20" s="3">
         <v>19</v>
       </c>
@@ -1565,11 +1568,11 @@
       <c r="D20" s="10" t="s">
         <v>59</v>
       </c>
-      <c r="E20" s="12" t="s">
+      <c r="E20" s="11" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="21" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" ht="56">
       <c r="A21" s="3">
         <v>20</v>
       </c>
@@ -1582,11 +1585,11 @@
       <c r="D21" s="10" t="s">
         <v>60</v>
       </c>
-      <c r="E21" s="12" t="s">
+      <c r="E21" s="11" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="22" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" ht="28">
       <c r="A22" s="3">
         <v>21</v>
       </c>
@@ -1597,7 +1600,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="23" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" ht="42">
       <c r="A23" s="3">
         <v>22</v>
       </c>
@@ -1610,11 +1613,11 @@
       <c r="D23" s="10" t="s">
         <v>61</v>
       </c>
-      <c r="E23" s="12" t="s">
+      <c r="E23" s="11" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="24" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" ht="56">
       <c r="A24" s="3">
         <v>23</v>
       </c>
@@ -1627,25 +1630,25 @@
       <c r="D24" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="E24" s="12" t="s">
+      <c r="E24" s="11" t="s">
         <v>83</v>
       </c>
       <c r="H24" s="3" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="26" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" ht="56">
       <c r="C26" s="7" t="s">
         <v>36</v>
       </c>
       <c r="D26" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="E26" s="12" t="s">
+      <c r="E26" s="11" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="28" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" ht="42">
       <c r="A28" s="3">
         <v>24</v>
       </c>
@@ -1659,7 +1662,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="29" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8" ht="56">
       <c r="A29" s="3">
         <v>25</v>
       </c>
@@ -1673,7 +1676,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="30" spans="1:8" ht="105" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8" ht="84">
       <c r="A30" s="3">
         <v>26</v>
       </c>
@@ -1686,29 +1689,29 @@
       <c r="D30" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="E30" s="12" t="s">
+      <c r="E30" s="11" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="31" spans="1:8" s="18" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A31" s="13">
+    <row r="31" spans="1:8" s="17" customFormat="1" ht="42">
+      <c r="A31" s="12">
         <v>27</v>
       </c>
-      <c r="B31" s="13" t="s">
+      <c r="B31" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="C31" s="14" t="s">
+      <c r="C31" s="13" t="s">
         <v>44</v>
       </c>
-      <c r="D31" s="15" t="s">
+      <c r="D31" s="14" t="s">
         <v>50</v>
       </c>
-      <c r="E31" s="16"/>
-      <c r="F31" s="13"/>
-      <c r="G31" s="13"/>
-      <c r="H31" s="17"/>
-    </row>
-    <row r="32" spans="1:8" ht="120" x14ac:dyDescent="0.25">
+      <c r="E31" s="15"/>
+      <c r="F31" s="12"/>
+      <c r="G31" s="12"/>
+      <c r="H31" s="16"/>
+    </row>
+    <row r="32" spans="1:8" ht="98">
       <c r="A32" s="3">
         <v>28</v>
       </c>
@@ -1721,11 +1724,11 @@
       <c r="D32" s="10" t="s">
         <v>49</v>
       </c>
-      <c r="E32" s="12" t="s">
+      <c r="E32" s="11" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="33" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:8" ht="56">
       <c r="A33" s="3">
         <v>29</v>
       </c>
@@ -1742,7 +1745,7 @@
       <c r="G33"/>
       <c r="H33"/>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:8">
       <c r="F36"/>
       <c r="G36"/>
       <c r="H36"/>
@@ -1753,7 +1756,7 @@
     <mergeCell ref="H8:H10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -1764,18 +1767,18 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:D13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="2" max="2" width="30.85546875" customWidth="1"/>
+    <col min="2" max="2" width="30.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -1783,7 +1786,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1791,12 +1794,17 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
         <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="D13" t="s">
+        <v>88</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
PROJECT REQUIREMENTS FOR 3/16/2015 - FOURTH ITERATION received Thursday, February 26, 2015 12:17 PM
</commit_message>
<xml_diff>
--- a/etc/pm/requirements/Pre-K Finder and Form Modifications 2015 - Round 2.xlsx
+++ b/etc/pm/requirements/Pre-K Finder and Form Modifications 2015 - Round 2.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25203"/>
-  <workbookPr autoCompressPictures="0"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24120" windowHeight="13620" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24120" windowHeight="13620"/>
   </bookViews>
   <sheets>
     <sheet name="Requirements" sheetId="1" r:id="rId1"/>
     <sheet name="Questions" sheetId="2" r:id="rId2"/>
+    <sheet name="Splash Page" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Requirements!$A$1:$H$11</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Requirements!$A$1:$I$11</definedName>
   </definedNames>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="140001"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -22,8 +23,42 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Keane, Tim</author>
+  </authors>
+  <commentList>
+    <comment ref="E17" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Keane, Tim:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Since the value for Charter School that will appear in PREK_TYPE has not been provided I am assuming it will be CHARTER.  Let's make it that in future data submissions.</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="108">
   <si>
     <t>Requirement</t>
   </si>
@@ -705,14 +740,71 @@
     <t>DP et al. responses</t>
   </si>
   <si>
-    <t>x</t>
+    <t>Initial View</t>
+  </si>
+  <si>
+    <t>Map View</t>
+  </si>
+  <si>
+    <t>provides room for descriptive text tobe provided by DOE.  Info icon as que to info button on map view.</t>
+  </si>
+  <si>
+    <t>Info button allows for the redisplay of the splash page.</t>
+  </si>
+  <si>
+    <t>Splash page redisplayed after clicking Info button.</t>
+  </si>
+  <si>
+    <t>seems redundant to have "Apply" and/or "Get in Touch" buttons on each school row and popup if they don’t do anything special.  One of each on the screen somplace makes more sense to me.  Either have them include the school with the form submission or get rid of school-specific buttons.</t>
+  </si>
+  <si>
+    <t>DoITT 2/26</t>
+  </si>
+  <si>
+    <t>OK</t>
+  </si>
+  <si>
+    <t>Ok</t>
+  </si>
+  <si>
+    <t>Ok. Moving forward, since this is a DOE form, edits should be made by DOE.</t>
+  </si>
+  <si>
+    <t>This rule doesn't caputure future years.  We will externalize the rule in a javascript file to be hosted at DOE that can be changed by DOE in the future.  We will send a file to for DOE to host in staging soon.</t>
+  </si>
+  <si>
+    <t>Screenshot of proposed design on "Splash Page" worksheet</t>
+  </si>
+  <si>
+    <t>We cannot code to future date without at least knowing what the schema will look like. What will be the value in the DAY_LENGTH field for 5 hour?</t>
+  </si>
+  <si>
+    <t>When will be receive the data?</t>
+  </si>
+  <si>
+    <t>We can design something that works.  Buit without a schema containing the names of fields for new values displayed in the mockup there is no way to even start on this.</t>
+  </si>
+  <si>
+    <t>Was meant to say "see comments on 17"… new note on 17 also applies here. We need the data now</t>
+  </si>
+  <si>
+    <t>Will be left for after 3/16</t>
+  </si>
+  <si>
+    <t>Meaning everything above is nice to have?</t>
+  </si>
+  <si>
+    <t>We will externalize the rule in a javascript file to be hosted at DOE that can be changed by DOE in the future.  We will send a file to for DOE to host in staging soon.</t>
+  </si>
+  <si>
+    <t>Splash screen is really the only workable solution.  Screenshot of proposed design on "Splash Page" worksheet.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -796,8 +888,36 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="20"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -807,6 +927,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -841,7 +967,7 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -892,8 +1018,32 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="19">
@@ -925,6 +1075,125 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>94857</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>75596</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1828800" y="1524000"/>
+          <a:ext cx="3142857" cy="4838096"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>94857</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>75596</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5486400" y="1524000"/>
+          <a:ext cx="3142857" cy="4838096"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>94857</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>75596</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7924800" y="1152525"/>
+          <a:ext cx="3142857" cy="4838096"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1213,28 +1482,29 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H36"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I36"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E2" sqref="E2"/>
+      <selection pane="bottomLeft" activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="5" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.5" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="67.33203125" style="4" customWidth="1"/>
-    <col min="4" max="4" width="46.33203125" style="10" customWidth="1"/>
-    <col min="5" max="5" width="46.33203125" style="11" customWidth="1"/>
-    <col min="6" max="6" width="8.5" style="3" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.5" style="3" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="64.1640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="67.28515625" style="4" customWidth="1"/>
+    <col min="4" max="4" width="46.28515625" style="10" customWidth="1"/>
+    <col min="5" max="5" width="46.28515625" style="11" customWidth="1"/>
+    <col min="6" max="6" width="46.28515625" style="25" customWidth="1"/>
+    <col min="7" max="7" width="8.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="64.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -1250,17 +1520,20 @@
       <c r="E1" s="7" t="s">
         <v>87</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="23" t="s">
+        <v>94</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="70">
+    <row r="2" spans="1:9" ht="105" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
         <v>1</v>
       </c>
@@ -1273,11 +1546,14 @@
       <c r="D2" s="10" t="s">
         <v>68</v>
       </c>
-      <c r="E2" s="11" t="s">
+      <c r="E2" s="18" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" ht="42">
+      <c r="F2" s="24" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <v>2</v>
       </c>
@@ -1287,8 +1563,11 @@
       <c r="C3" s="4" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="4" spans="1:8">
+      <c r="F3" s="25" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
         <v>3</v>
       </c>
@@ -1298,8 +1577,11 @@
       <c r="C4" s="4" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" ht="56">
+      <c r="F4" s="25" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
         <v>4</v>
       </c>
@@ -1312,13 +1594,16 @@
       <c r="D5" s="10" t="s">
         <v>63</v>
       </c>
-      <c r="E5" s="11" t="s">
+      <c r="E5" s="18" t="s">
         <v>70</v>
       </c>
-      <c r="G5" s="5"/>
+      <c r="F5" s="24" t="s">
+        <v>95</v>
+      </c>
       <c r="H5" s="5"/>
-    </row>
-    <row r="6" spans="1:8" ht="42">
+      <c r="I5" s="5"/>
+    </row>
+    <row r="6" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
         <v>5</v>
       </c>
@@ -1334,12 +1619,12 @@
       <c r="E6" s="11" t="s">
         <v>71</v>
       </c>
-      <c r="G6" s="5"/>
-      <c r="H6" s="9" t="s">
+      <c r="H6" s="5"/>
+      <c r="I6" s="9" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="56">
+    <row r="7" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
         <v>6</v>
       </c>
@@ -1352,11 +1637,14 @@
       <c r="D7" s="10" t="s">
         <v>65</v>
       </c>
-      <c r="E7" s="11" t="s">
+      <c r="E7" s="18" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" ht="70">
+      <c r="F7" s="24" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="90" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
         <v>7</v>
       </c>
@@ -1372,11 +1660,14 @@
       <c r="E8" s="11" t="s">
         <v>73</v>
       </c>
-      <c r="H8" s="18" t="s">
+      <c r="F8" s="25" t="s">
+        <v>95</v>
+      </c>
+      <c r="I8" s="20" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="28">
+    <row r="9" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
         <v>8</v>
       </c>
@@ -1389,12 +1680,15 @@
       <c r="D9" s="10" t="s">
         <v>66</v>
       </c>
-      <c r="E9" s="11" t="s">
+      <c r="E9" s="18" t="s">
         <v>74</v>
       </c>
-      <c r="H9" s="18"/>
-    </row>
-    <row r="10" spans="1:8">
+      <c r="F9" s="24" t="s">
+        <v>98</v>
+      </c>
+      <c r="I9" s="20"/>
+    </row>
+    <row r="10" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
         <v>9</v>
       </c>
@@ -1404,9 +1698,12 @@
       <c r="C10" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="H10" s="18"/>
-    </row>
-    <row r="11" spans="1:8" ht="28">
+      <c r="F10" s="25" t="s">
+        <v>95</v>
+      </c>
+      <c r="I10" s="20"/>
+    </row>
+    <row r="11" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="3">
         <v>10</v>
       </c>
@@ -1416,8 +1713,11 @@
       <c r="C11" s="4" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="12" spans="1:8" ht="56">
+      <c r="F11" s="25" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A12" s="3">
         <v>11</v>
       </c>
@@ -1427,8 +1727,11 @@
       <c r="C12" s="4" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="13" spans="1:8" ht="28">
+      <c r="F12" s="25" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="3">
         <v>12</v>
       </c>
@@ -1438,13 +1741,16 @@
       <c r="C13" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="F13"/>
+      <c r="F13" s="25" t="s">
+        <v>95</v>
+      </c>
       <c r="G13"/>
-      <c r="H13" t="s">
+      <c r="H13"/>
+      <c r="I13" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="28">
+    <row r="14" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="3">
         <v>13</v>
       </c>
@@ -1460,11 +1766,14 @@
       <c r="E14" s="11" t="s">
         <v>75</v>
       </c>
-      <c r="F14"/>
+      <c r="F14" s="25" t="s">
+        <v>95</v>
+      </c>
       <c r="G14"/>
       <c r="H14"/>
-    </row>
-    <row r="15" spans="1:8" ht="56">
+      <c r="I14"/>
+    </row>
+    <row r="15" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A15" s="3">
         <v>14</v>
       </c>
@@ -1477,11 +1786,14 @@
       <c r="D15" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="E15" s="11" t="s">
+      <c r="E15" s="18" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="16" spans="1:8" ht="70">
+      <c r="F15" s="24" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A16" s="3">
         <v>15</v>
       </c>
@@ -1494,11 +1806,14 @@
       <c r="D16" s="10" t="s">
         <v>52</v>
       </c>
-      <c r="E16" s="11" t="s">
+      <c r="E16" s="18" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="17" spans="1:8" s="17" customFormat="1" ht="70">
+      <c r="F16" s="24" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" s="17" customFormat="1" ht="90" x14ac:dyDescent="0.25">
       <c r="A17" s="12">
         <v>16</v>
       </c>
@@ -1514,11 +1829,14 @@
       <c r="E17" s="15" t="s">
         <v>78</v>
       </c>
-      <c r="F17" s="12"/>
+      <c r="F17" s="26" t="s">
+        <v>101</v>
+      </c>
       <c r="G17" s="12"/>
-      <c r="H17" s="16"/>
-    </row>
-    <row r="18" spans="1:8" ht="98">
+      <c r="H17" s="12"/>
+      <c r="I17" s="16"/>
+    </row>
+    <row r="18" spans="1:9" ht="135" x14ac:dyDescent="0.25">
       <c r="A18" s="3">
         <v>17</v>
       </c>
@@ -1531,14 +1849,17 @@
       <c r="D18" s="10" t="s">
         <v>53</v>
       </c>
-      <c r="E18" s="11" t="s">
+      <c r="E18" s="18" t="s">
         <v>79</v>
       </c>
-      <c r="H18" s="8" t="s">
+      <c r="F18" s="24" t="s">
+        <v>102</v>
+      </c>
+      <c r="I18" s="8" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="19" spans="1:8" ht="28">
+    <row r="19" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A19" s="3">
         <v>18</v>
       </c>
@@ -1551,11 +1872,14 @@
       <c r="D19" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="E19" s="11" t="s">
+      <c r="E19" s="18" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="20" spans="1:8" ht="70">
+      <c r="F19" s="24" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" ht="90" x14ac:dyDescent="0.25">
       <c r="A20" s="3">
         <v>19</v>
       </c>
@@ -1572,7 +1896,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="21" spans="1:8" ht="56">
+    <row r="21" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A21" s="3">
         <v>20</v>
       </c>
@@ -1589,7 +1913,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="22" spans="1:8" ht="28">
+    <row r="22" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A22" s="3">
         <v>21</v>
       </c>
@@ -1600,7 +1924,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="23" spans="1:8" ht="42">
+    <row r="23" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A23" s="3">
         <v>22</v>
       </c>
@@ -1617,7 +1941,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="24" spans="1:8" ht="56">
+    <row r="24" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A24" s="3">
         <v>23</v>
       </c>
@@ -1630,25 +1954,31 @@
       <c r="D24" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="E24" s="11" t="s">
+      <c r="E24" s="18" t="s">
         <v>83</v>
       </c>
-      <c r="H24" s="3" t="s">
+      <c r="F24" s="24" t="s">
+        <v>104</v>
+      </c>
+      <c r="I24" s="3" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="26" spans="1:8" ht="56">
+    <row r="26" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="C26" s="7" t="s">
         <v>36</v>
       </c>
       <c r="D26" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="E26" s="11" t="s">
+      <c r="E26" s="18" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="28" spans="1:8" ht="42">
+      <c r="F26" s="24" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A28" s="3">
         <v>24</v>
       </c>
@@ -1661,8 +1991,11 @@
       <c r="D28" s="10" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="29" spans="1:8" ht="56">
+      <c r="F28" s="24" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A29" s="3">
         <v>25</v>
       </c>
@@ -1675,8 +2008,11 @@
       <c r="D29" s="10" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="30" spans="1:8" ht="84">
+      <c r="F29" s="24" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" ht="105" x14ac:dyDescent="0.25">
       <c r="A30" s="3">
         <v>26</v>
       </c>
@@ -1689,11 +2025,14 @@
       <c r="D30" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="E30" s="11" t="s">
+      <c r="E30" s="18" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="31" spans="1:8" s="17" customFormat="1" ht="42">
+      <c r="F30" s="24" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" s="17" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A31" s="12">
         <v>27</v>
       </c>
@@ -1707,11 +2046,12 @@
         <v>50</v>
       </c>
       <c r="E31" s="15"/>
-      <c r="F31" s="12"/>
+      <c r="F31" s="26"/>
       <c r="G31" s="12"/>
-      <c r="H31" s="16"/>
-    </row>
-    <row r="32" spans="1:8" ht="98">
+      <c r="H31" s="12"/>
+      <c r="I31" s="16"/>
+    </row>
+    <row r="32" spans="1:9" ht="120" x14ac:dyDescent="0.25">
       <c r="A32" s="3">
         <v>28</v>
       </c>
@@ -1724,11 +2064,14 @@
       <c r="D32" s="10" t="s">
         <v>49</v>
       </c>
-      <c r="E32" s="11" t="s">
+      <c r="E32" s="18" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="33" spans="1:8" ht="56">
+      <c r="F32" s="24" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A33" s="3">
         <v>29</v>
       </c>
@@ -1741,22 +2084,23 @@
       <c r="D33" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="F33"/>
       <c r="G33"/>
       <c r="H33"/>
-    </row>
-    <row r="36" spans="1:8">
-      <c r="F36"/>
+      <c r="I33"/>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="G36"/>
       <c r="H36"/>
+      <c r="I36"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:H11"/>
+  <autoFilter ref="A1:I11"/>
   <mergeCells count="1">
-    <mergeCell ref="H8:H10"/>
+    <mergeCell ref="I8:I10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait"/>
+  <pageSetup paperSize="3" orientation="landscape" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -1767,18 +2111,18 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D13"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="30.83203125" customWidth="1"/>
+    <col min="2" max="2" width="30.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -1786,7 +2130,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1794,17 +2138,12 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
         <v>4</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4">
-      <c r="D13" t="s">
-        <v>88</v>
       </c>
     </row>
   </sheetData>
@@ -1815,4 +2154,82 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:R3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3:F3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="5.85546875" customWidth="1"/>
+    <col min="7" max="7" width="5.85546875" customWidth="1"/>
+    <col min="13" max="13" width="5.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:18" ht="28.5" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B2" s="21" t="s">
+        <v>88</v>
+      </c>
+      <c r="C2" s="22"/>
+      <c r="D2" s="22"/>
+      <c r="E2" s="22"/>
+      <c r="F2" s="22"/>
+      <c r="H2" s="21" t="s">
+        <v>89</v>
+      </c>
+      <c r="I2" s="22"/>
+      <c r="J2" s="22"/>
+      <c r="K2" s="22"/>
+      <c r="L2" s="22"/>
+      <c r="N2" s="21" t="s">
+        <v>89</v>
+      </c>
+      <c r="O2" s="22"/>
+      <c r="P2" s="22"/>
+      <c r="Q2" s="22"/>
+      <c r="R2" s="22"/>
+    </row>
+    <row r="3" spans="2:18" ht="58.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="20" t="s">
+        <v>90</v>
+      </c>
+      <c r="C3" s="20"/>
+      <c r="D3" s="20"/>
+      <c r="E3" s="20"/>
+      <c r="F3" s="20"/>
+      <c r="G3" s="19"/>
+      <c r="H3" s="20" t="s">
+        <v>91</v>
+      </c>
+      <c r="I3" s="20"/>
+      <c r="J3" s="20"/>
+      <c r="K3" s="20"/>
+      <c r="L3" s="20"/>
+      <c r="M3" s="19"/>
+      <c r="N3" s="20" t="s">
+        <v>92</v>
+      </c>
+      <c r="O3" s="20"/>
+      <c r="P3" s="20"/>
+      <c r="Q3" s="20"/>
+      <c r="R3" s="20"/>
+    </row>
+  </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="B3:F3"/>
+    <mergeCell ref="B2:F2"/>
+    <mergeCell ref="H2:L2"/>
+    <mergeCell ref="H3:L3"/>
+    <mergeCell ref="N2:R2"/>
+    <mergeCell ref="N3:R3"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
PROJECT REQUIREMENTS FOR 3/16/2015 - SIXTH ITERATION received Friday, February 27, 2015 7:30 PM
</commit_message>
<xml_diff>
--- a/etc/pm/requirements/Pre-K Finder and Form Modifications 2015 - Round 2.xlsx
+++ b/etc/pm/requirements/Pre-K Finder and Form Modifications 2015 - Round 2.xlsx
@@ -12,7 +12,7 @@
     <sheet name="Splash Page" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Requirements!$A$1:$I$11</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Requirements!$A$1:$J$11</definedName>
   </definedNames>
   <calcPr calcId="140001"/>
   <extLst>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="121">
   <si>
     <t>Requirement</t>
   </si>
@@ -798,6 +798,45 @@
   </si>
   <si>
     <t>Splash screen is really the only workable solution.  Screenshot of proposed design on "Splash Page" worksheet.</t>
+  </si>
+  <si>
+    <t>Per 02/26 meeting</t>
+  </si>
+  <si>
+    <t>ok - all required fields needed to submit</t>
+  </si>
+  <si>
+    <t>ok on splash page.  DOE providing text and button color suggestions.</t>
+  </si>
+  <si>
+    <t>Data being provided by DOE</t>
+  </si>
+  <si>
+    <t>Sample data COB 02/27 from DOE</t>
+  </si>
+  <si>
+    <t>Sample data COB 02/27 from DOE.  OK on keeping details in the slidedown.</t>
+  </si>
+  <si>
+    <t>TBD.  A nice to have if possible.</t>
+  </si>
+  <si>
+    <t>Using "NOTE" field to capture this (or any other) information we want to display about the site.  Color of text TBD.</t>
+  </si>
+  <si>
+    <t>ok, possiblly for post 3/16</t>
+  </si>
+  <si>
+    <t>DIIT team to do.  Slight modification of text coming from DOE.</t>
+  </si>
+  <si>
+    <t>ok - not clear if this is to put in place for future years or if javascript file needed for March 16th this year</t>
+  </si>
+  <si>
+    <t>DOE to provide replacement text for the bottom of the form</t>
+  </si>
+  <si>
+    <t>DoiTT to change from Search by "School" to Search by "Program"</t>
   </si>
 </sst>
 </file>
@@ -937,12 +976,27 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -967,60 +1021,8 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -1033,17 +1035,73 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="19">
@@ -1483,620 +1541,713 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I36"/>
+  <dimension ref="A1:J36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H4" sqref="H4"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.42578125" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="67.28515625" style="4" customWidth="1"/>
-    <col min="4" max="4" width="46.28515625" style="10" customWidth="1"/>
-    <col min="5" max="5" width="46.28515625" style="11" customWidth="1"/>
-    <col min="6" max="6" width="46.28515625" style="25" customWidth="1"/>
-    <col min="7" max="7" width="8.42578125" style="3" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.42578125" style="3" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="64.140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5" style="10" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.42578125" style="10" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="67.28515625" style="11" customWidth="1"/>
+    <col min="4" max="4" width="46.28515625" style="12" customWidth="1"/>
+    <col min="5" max="5" width="46.28515625" style="15" customWidth="1"/>
+    <col min="6" max="7" width="46.28515625" style="16" customWidth="1"/>
+    <col min="8" max="8" width="8.42578125" style="10" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.42578125" style="10" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="64.140625" style="10" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8.85546875" style="9"/>
+    <col min="12" max="12" width="11.42578125" style="9" bestFit="1" customWidth="1"/>
+    <col min="13" max="16384" width="8.85546875" style="9"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="6" t="s">
         <v>54</v>
       </c>
       <c r="E1" s="7" t="s">
         <v>87</v>
       </c>
-      <c r="F1" s="23" t="s">
+      <c r="F1" s="8" t="s">
         <v>94</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="8" t="s">
+        <v>108</v>
+      </c>
+      <c r="H1" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="5" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="105" x14ac:dyDescent="0.25">
-      <c r="A2" s="3">
+    <row r="2" spans="1:10" ht="105" x14ac:dyDescent="0.25">
+      <c r="A2" s="10">
         <v>1</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="D2" s="10" t="s">
+      <c r="D2" s="12" t="s">
         <v>68</v>
       </c>
-      <c r="E2" s="18" t="s">
+      <c r="E2" s="13" t="s">
         <v>69</v>
       </c>
-      <c r="F2" s="24" t="s">
+      <c r="F2" s="14" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" ht="60" x14ac:dyDescent="0.25">
-      <c r="A3" s="3">
+      <c r="G2" s="14" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+      <c r="A3" s="10">
         <v>2</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="F3" s="25" t="s">
+      <c r="F3" s="16" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="3">
+      <c r="G3" s="16" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" s="10">
         <v>3</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="F4" s="25" t="s">
+      <c r="F4" s="16" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" ht="75" x14ac:dyDescent="0.25">
-      <c r="A5" s="3">
+      <c r="G4" s="16" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="75" x14ac:dyDescent="0.25">
+      <c r="A5" s="10">
         <v>4</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C5" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="D5" s="10" t="s">
+      <c r="D5" s="12" t="s">
         <v>63</v>
       </c>
-      <c r="E5" s="18" t="s">
+      <c r="E5" s="13" t="s">
         <v>70</v>
       </c>
-      <c r="F5" s="24" t="s">
+      <c r="F5" s="14" t="s">
         <v>95</v>
       </c>
-      <c r="H5" s="5"/>
-      <c r="I5" s="5"/>
-    </row>
-    <row r="6" spans="1:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="A6" s="3">
+      <c r="G5" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="I5" s="17"/>
+      <c r="J5" s="17"/>
+    </row>
+    <row r="6" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="A6" s="10">
         <v>5</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="C6" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="D6" s="10" t="s">
+      <c r="D6" s="12" t="s">
         <v>64</v>
       </c>
-      <c r="E6" s="11" t="s">
+      <c r="E6" s="15" t="s">
         <v>71</v>
       </c>
-      <c r="H6" s="5"/>
-      <c r="I6" s="9" t="s">
+      <c r="G6" s="16" t="s">
+        <v>81</v>
+      </c>
+      <c r="I6" s="17"/>
+      <c r="J6" s="18" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="75" x14ac:dyDescent="0.25">
-      <c r="A7" s="3">
+    <row r="7" spans="1:10" ht="75" x14ac:dyDescent="0.25">
+      <c r="A7" s="10">
         <v>6</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B7" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="4" t="s">
+      <c r="C7" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="D7" s="10" t="s">
+      <c r="D7" s="12" t="s">
         <v>65</v>
       </c>
-      <c r="E7" s="18" t="s">
+      <c r="E7" s="13" t="s">
         <v>72</v>
       </c>
-      <c r="F7" s="24" t="s">
+      <c r="F7" s="14" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" ht="90" x14ac:dyDescent="0.25">
-      <c r="A8" s="3">
+      <c r="G7" s="14" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" ht="90" x14ac:dyDescent="0.25">
+      <c r="A8" s="10">
         <v>7</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="B8" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="4" t="s">
+      <c r="C8" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="D8" s="10" t="s">
+      <c r="D8" s="12" t="s">
         <v>67</v>
       </c>
-      <c r="E8" s="11" t="s">
+      <c r="E8" s="15" t="s">
         <v>73</v>
       </c>
-      <c r="F8" s="25" t="s">
+      <c r="F8" s="16" t="s">
         <v>95</v>
       </c>
-      <c r="I8" s="20" t="s">
+      <c r="G8" s="16" t="s">
+        <v>81</v>
+      </c>
+      <c r="J8" s="19" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="75" x14ac:dyDescent="0.25">
-      <c r="A9" s="3">
+    <row r="9" spans="1:10" ht="75" x14ac:dyDescent="0.25">
+      <c r="A9" s="10">
         <v>8</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="B9" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="C9" s="6" t="s">
+      <c r="C9" s="20" t="s">
         <v>13</v>
       </c>
-      <c r="D9" s="10" t="s">
+      <c r="D9" s="12" t="s">
         <v>66</v>
       </c>
-      <c r="E9" s="18" t="s">
+      <c r="E9" s="13" t="s">
         <v>74</v>
       </c>
-      <c r="F9" s="24" t="s">
+      <c r="F9" s="14" t="s">
         <v>98</v>
       </c>
-      <c r="I9" s="20"/>
-    </row>
-    <row r="10" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A10" s="3">
+      <c r="G9" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="J9" s="19"/>
+    </row>
+    <row r="10" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10" s="10">
         <v>9</v>
       </c>
-      <c r="B10" s="3" t="s">
+      <c r="B10" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="C10" s="6" t="s">
+      <c r="C10" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="F10" s="25" t="s">
+      <c r="F10" s="16" t="s">
         <v>95</v>
       </c>
-      <c r="I10" s="20"/>
-    </row>
-    <row r="11" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A11" s="3">
+      <c r="G10" s="16" t="s">
+        <v>81</v>
+      </c>
+      <c r="J10" s="19"/>
+    </row>
+    <row r="11" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A11" s="10">
         <v>10</v>
       </c>
-      <c r="B11" s="3" t="s">
+      <c r="B11" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="C11" s="4" t="s">
+      <c r="C11" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="F11" s="25" t="s">
+      <c r="F11" s="16" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="12" spans="1:9" ht="75" x14ac:dyDescent="0.25">
-      <c r="A12" s="3">
+      <c r="G11" s="16" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" ht="75" x14ac:dyDescent="0.25">
+      <c r="A12" s="10">
         <v>11</v>
       </c>
-      <c r="B12" s="3" t="s">
+      <c r="B12" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="C12" s="4" t="s">
+      <c r="C12" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="F12" s="25" t="s">
+      <c r="F12" s="16" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="13" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A13" s="3">
+      <c r="G12" s="16" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A13" s="10">
         <v>12</v>
       </c>
-      <c r="B13" s="3" t="s">
+      <c r="B13" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="C13" s="4" t="s">
+      <c r="C13" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="F13" s="25" t="s">
+      <c r="F13" s="16" t="s">
         <v>95</v>
       </c>
-      <c r="G13"/>
-      <c r="H13"/>
-      <c r="I13" t="s">
+      <c r="G13" s="16" t="s">
+        <v>81</v>
+      </c>
+      <c r="H13" s="9"/>
+      <c r="I13" s="9"/>
+      <c r="J13" s="9" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A14" s="3">
+    <row r="14" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A14" s="10">
         <v>13</v>
       </c>
-      <c r="B14" s="3" t="s">
+      <c r="B14" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="C14" s="4" t="s">
+      <c r="C14" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="D14" s="10" t="s">
+      <c r="D14" s="12" t="s">
         <v>56</v>
       </c>
-      <c r="E14" s="11" t="s">
+      <c r="E14" s="15" t="s">
         <v>75</v>
       </c>
-      <c r="F14" s="25" t="s">
+      <c r="F14" s="16" t="s">
         <v>95</v>
       </c>
-      <c r="G14"/>
-      <c r="H14"/>
-      <c r="I14"/>
-    </row>
-    <row r="15" spans="1:9" ht="75" x14ac:dyDescent="0.25">
-      <c r="A15" s="3">
+      <c r="G14" s="16" t="s">
+        <v>81</v>
+      </c>
+      <c r="H14" s="9"/>
+      <c r="I14" s="9"/>
+      <c r="J14" s="9"/>
+    </row>
+    <row r="15" spans="1:10" ht="75" x14ac:dyDescent="0.25">
+      <c r="A15" s="10">
         <v>14</v>
       </c>
-      <c r="B15" s="3" t="s">
+      <c r="B15" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="C15" s="4" t="s">
+      <c r="C15" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="D15" s="10" t="s">
+      <c r="D15" s="12" t="s">
         <v>57</v>
       </c>
-      <c r="E15" s="18" t="s">
+      <c r="E15" s="13" t="s">
         <v>77</v>
       </c>
-      <c r="F15" s="24" t="s">
+      <c r="F15" s="14" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="16" spans="1:9" ht="75" x14ac:dyDescent="0.25">
-      <c r="A16" s="3">
+      <c r="G15" s="14" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" ht="75" x14ac:dyDescent="0.25">
+      <c r="A16" s="10">
         <v>15</v>
       </c>
-      <c r="B16" s="3" t="s">
+      <c r="B16" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="C16" s="4" t="s">
+      <c r="C16" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="D16" s="10" t="s">
+      <c r="D16" s="12" t="s">
         <v>52</v>
       </c>
-      <c r="E16" s="18" t="s">
+      <c r="E16" s="13" t="s">
         <v>76</v>
       </c>
-      <c r="F16" s="24" t="s">
+      <c r="F16" s="14" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="17" spans="1:9" s="17" customFormat="1" ht="90" x14ac:dyDescent="0.25">
-      <c r="A17" s="12">
+      <c r="G16" s="14" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" s="27" customFormat="1" ht="90" x14ac:dyDescent="0.25">
+      <c r="A17" s="21">
         <v>16</v>
       </c>
-      <c r="B17" s="12" t="s">
+      <c r="B17" s="21" t="s">
         <v>24</v>
       </c>
-      <c r="C17" s="13" t="s">
+      <c r="C17" s="22" t="s">
         <v>39</v>
       </c>
-      <c r="D17" s="14" t="s">
+      <c r="D17" s="23" t="s">
         <v>55</v>
       </c>
-      <c r="E17" s="15" t="s">
+      <c r="E17" s="24" t="s">
         <v>78</v>
       </c>
-      <c r="F17" s="26" t="s">
+      <c r="F17" s="25" t="s">
         <v>101</v>
       </c>
-      <c r="G17" s="12"/>
-      <c r="H17" s="12"/>
-      <c r="I17" s="16"/>
-    </row>
-    <row r="18" spans="1:9" ht="135" x14ac:dyDescent="0.25">
-      <c r="A18" s="3">
+      <c r="G17" s="25" t="s">
+        <v>112</v>
+      </c>
+      <c r="H17" s="21"/>
+      <c r="I17" s="21"/>
+      <c r="J17" s="26"/>
+    </row>
+    <row r="18" spans="1:10" ht="135" x14ac:dyDescent="0.25">
+      <c r="A18" s="10">
         <v>17</v>
       </c>
-      <c r="B18" s="3" t="s">
+      <c r="B18" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="C18" s="4" t="s">
+      <c r="C18" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="D18" s="10" t="s">
+      <c r="D18" s="12" t="s">
         <v>53</v>
       </c>
-      <c r="E18" s="18" t="s">
+      <c r="E18" s="13" t="s">
         <v>79</v>
       </c>
-      <c r="F18" s="24" t="s">
+      <c r="F18" s="14" t="s">
         <v>102</v>
       </c>
-      <c r="I18" s="8" t="s">
+      <c r="G18" s="14" t="s">
+        <v>113</v>
+      </c>
+      <c r="J18" s="28" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="19" spans="1:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="A19" s="3">
+    <row r="19" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="A19" s="10">
         <v>18</v>
       </c>
-      <c r="B19" s="3" t="s">
+      <c r="B19" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="C19" s="4" t="s">
+      <c r="C19" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="D19" s="10" t="s">
+      <c r="D19" s="12" t="s">
         <v>58</v>
       </c>
-      <c r="E19" s="18" t="s">
+      <c r="E19" s="13" t="s">
         <v>80</v>
       </c>
-      <c r="F19" s="24" t="s">
+      <c r="F19" s="14" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="20" spans="1:9" ht="90" x14ac:dyDescent="0.25">
-      <c r="A20" s="3">
+      <c r="G19" s="14" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" ht="90" x14ac:dyDescent="0.25">
+      <c r="A20" s="10">
         <v>19</v>
       </c>
-      <c r="B20" s="3" t="s">
+      <c r="B20" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="C20" s="4" t="s">
+      <c r="C20" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="D20" s="10" t="s">
+      <c r="D20" s="12" t="s">
         <v>59</v>
       </c>
-      <c r="E20" s="11" t="s">
+      <c r="E20" s="15" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="21" spans="1:9" ht="75" x14ac:dyDescent="0.25">
-      <c r="A21" s="3">
+      <c r="G20" s="16" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" ht="75" x14ac:dyDescent="0.25">
+      <c r="A21" s="10">
         <v>20</v>
       </c>
-      <c r="B21" s="3" t="s">
+      <c r="B21" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="C21" s="4" t="s">
+      <c r="C21" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="D21" s="10" t="s">
+      <c r="D21" s="12" t="s">
         <v>60</v>
       </c>
-      <c r="E21" s="11" t="s">
+      <c r="E21" s="15" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="22" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A22" s="3">
+      <c r="G21" s="16" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A22" s="10">
         <v>21</v>
       </c>
-      <c r="B22" s="3" t="s">
+      <c r="B22" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="C22" s="4" t="s">
+      <c r="C22" s="11" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="23" spans="1:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="A23" s="3">
+      <c r="G22" s="16" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="A23" s="10">
         <v>22</v>
       </c>
-      <c r="B23" s="3" t="s">
+      <c r="B23" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="C23" s="4" t="s">
+      <c r="C23" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="D23" s="10" t="s">
+      <c r="D23" s="12" t="s">
         <v>61</v>
       </c>
-      <c r="E23" s="11" t="s">
+      <c r="E23" s="15" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="24" spans="1:9" ht="60" x14ac:dyDescent="0.25">
-      <c r="A24" s="3">
+      <c r="G23" s="16" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+      <c r="A24" s="10">
         <v>23</v>
       </c>
-      <c r="B24" s="3" t="s">
+      <c r="B24" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="C24" s="4" t="s">
+      <c r="C24" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="D24" s="10" t="s">
+      <c r="D24" s="12" t="s">
         <v>47</v>
       </c>
-      <c r="E24" s="18" t="s">
+      <c r="E24" s="13" t="s">
         <v>83</v>
       </c>
-      <c r="F24" s="24" t="s">
+      <c r="F24" s="14" t="s">
         <v>104</v>
       </c>
-      <c r="I24" s="3" t="s">
+      <c r="G24" s="14" t="s">
+        <v>116</v>
+      </c>
+      <c r="J24" s="10" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="26" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="C26" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="D26" s="10" t="s">
+      <c r="D26" s="12" t="s">
         <v>48</v>
       </c>
-      <c r="E26" s="18" t="s">
+      <c r="E26" s="13" t="s">
         <v>84</v>
       </c>
-      <c r="F26" s="24" t="s">
+      <c r="F26" s="14" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="28" spans="1:9" ht="60" x14ac:dyDescent="0.25">
-      <c r="A28" s="3">
+      <c r="G26" s="14"/>
+    </row>
+    <row r="28" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+      <c r="A28" s="10">
         <v>24</v>
       </c>
-      <c r="B28" s="3" t="s">
+      <c r="B28" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="C28" s="4" t="s">
+      <c r="C28" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="D28" s="10" t="s">
+      <c r="D28" s="12" t="s">
         <v>62</v>
       </c>
-      <c r="F28" s="24" t="s">
+      <c r="F28" s="14" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="29" spans="1:9" ht="75" x14ac:dyDescent="0.25">
-      <c r="A29" s="3">
+      <c r="G28" s="14" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" ht="75" x14ac:dyDescent="0.25">
+      <c r="A29" s="10">
         <v>25</v>
       </c>
-      <c r="B29" s="3" t="s">
+      <c r="B29" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="C29" s="4" t="s">
+      <c r="C29" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="D29" s="10" t="s">
+      <c r="D29" s="12" t="s">
         <v>62</v>
       </c>
-      <c r="F29" s="24" t="s">
+      <c r="F29" s="14" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="30" spans="1:9" ht="105" x14ac:dyDescent="0.25">
-      <c r="A30" s="3">
+      <c r="G29" s="14" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" ht="105" x14ac:dyDescent="0.25">
+      <c r="A30" s="10">
         <v>26</v>
       </c>
-      <c r="B30" s="3" t="s">
+      <c r="B30" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="C30" s="4" t="s">
+      <c r="C30" s="11" t="s">
         <v>43</v>
       </c>
-      <c r="D30" s="10" t="s">
+      <c r="D30" s="12" t="s">
         <v>51</v>
       </c>
-      <c r="E30" s="18" t="s">
+      <c r="E30" s="13" t="s">
         <v>86</v>
       </c>
-      <c r="F30" s="24" t="s">
+      <c r="F30" s="14" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="31" spans="1:9" s="17" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A31" s="12">
+      <c r="G30" s="14" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" s="27" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A31" s="21">
         <v>27</v>
       </c>
-      <c r="B31" s="12" t="s">
+      <c r="B31" s="21" t="s">
         <v>24</v>
       </c>
-      <c r="C31" s="13" t="s">
+      <c r="C31" s="22" t="s">
         <v>44</v>
       </c>
-      <c r="D31" s="14" t="s">
+      <c r="D31" s="23" t="s">
         <v>50</v>
       </c>
-      <c r="E31" s="15"/>
-      <c r="F31" s="26"/>
-      <c r="G31" s="12"/>
-      <c r="H31" s="12"/>
-      <c r="I31" s="16"/>
-    </row>
-    <row r="32" spans="1:9" ht="120" x14ac:dyDescent="0.25">
-      <c r="A32" s="3">
+      <c r="E31" s="24"/>
+      <c r="F31" s="25"/>
+      <c r="G31" s="25" t="s">
+        <v>81</v>
+      </c>
+      <c r="H31" s="21"/>
+      <c r="I31" s="21"/>
+      <c r="J31" s="26"/>
+    </row>
+    <row r="32" spans="1:10" ht="120" x14ac:dyDescent="0.25">
+      <c r="A32" s="10">
         <v>28</v>
       </c>
-      <c r="B32" s="3" t="s">
+      <c r="B32" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="C32" s="4" t="s">
+      <c r="C32" s="11" t="s">
         <v>45</v>
       </c>
-      <c r="D32" s="10" t="s">
+      <c r="D32" s="12" t="s">
         <v>49</v>
       </c>
-      <c r="E32" s="18" t="s">
+      <c r="E32" s="13" t="s">
         <v>85</v>
       </c>
-      <c r="F32" s="24" t="s">
+      <c r="F32" s="14" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="33" spans="1:9" ht="75" x14ac:dyDescent="0.25">
-      <c r="A33" s="3">
+      <c r="G32" s="14" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" ht="75" x14ac:dyDescent="0.25">
+      <c r="A33" s="10">
         <v>29</v>
       </c>
-      <c r="B33" s="3" t="s">
+      <c r="B33" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="C33" s="4" t="s">
+      <c r="C33" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="D33" s="10" t="s">
+      <c r="D33" s="12" t="s">
         <v>50</v>
       </c>
-      <c r="G33"/>
-      <c r="H33"/>
-      <c r="I33"/>
-    </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="G36"/>
-      <c r="H36"/>
-      <c r="I36"/>
+      <c r="G33" s="16" t="s">
+        <v>81</v>
+      </c>
+      <c r="H33" s="9"/>
+      <c r="I33" s="9"/>
+      <c r="J33" s="9"/>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="H36" s="9"/>
+      <c r="I36" s="9"/>
+      <c r="J36" s="9"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:I11"/>
+  <autoFilter ref="A1:J11"/>
   <mergeCells count="1">
-    <mergeCell ref="I8:I10"/>
+    <mergeCell ref="J8:J10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="3" orientation="landscape" r:id="rId1"/>
@@ -2172,52 +2323,52 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:18" ht="28.5" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B2" s="21" t="s">
+      <c r="B2" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="C2" s="22"/>
-      <c r="D2" s="22"/>
-      <c r="E2" s="22"/>
-      <c r="F2" s="22"/>
-      <c r="H2" s="21" t="s">
+      <c r="C2" s="4"/>
+      <c r="D2" s="4"/>
+      <c r="E2" s="4"/>
+      <c r="F2" s="4"/>
+      <c r="H2" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="I2" s="22"/>
-      <c r="J2" s="22"/>
-      <c r="K2" s="22"/>
-      <c r="L2" s="22"/>
-      <c r="N2" s="21" t="s">
+      <c r="I2" s="4"/>
+      <c r="J2" s="4"/>
+      <c r="K2" s="4"/>
+      <c r="L2" s="4"/>
+      <c r="N2" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="O2" s="22"/>
-      <c r="P2" s="22"/>
-      <c r="Q2" s="22"/>
-      <c r="R2" s="22"/>
+      <c r="O2" s="4"/>
+      <c r="P2" s="4"/>
+      <c r="Q2" s="4"/>
+      <c r="R2" s="4"/>
     </row>
     <row r="3" spans="2:18" ht="58.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="20" t="s">
+      <c r="B3" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="C3" s="20"/>
-      <c r="D3" s="20"/>
-      <c r="E3" s="20"/>
-      <c r="F3" s="20"/>
-      <c r="G3" s="19"/>
-      <c r="H3" s="20" t="s">
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="I3" s="20"/>
-      <c r="J3" s="20"/>
-      <c r="K3" s="20"/>
-      <c r="L3" s="20"/>
-      <c r="M3" s="19"/>
-      <c r="N3" s="20" t="s">
+      <c r="I3" s="2"/>
+      <c r="J3" s="2"/>
+      <c r="K3" s="2"/>
+      <c r="L3" s="2"/>
+      <c r="M3" s="1"/>
+      <c r="N3" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="O3" s="20"/>
-      <c r="P3" s="20"/>
-      <c r="Q3" s="20"/>
-      <c r="R3" s="20"/>
+      <c r="O3" s="2"/>
+      <c r="P3" s="2"/>
+      <c r="Q3" s="2"/>
+      <c r="R3" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="6">

</xml_diff>

<commit_message>
PROJECT REQUIREMENTS FOR 3/16/2015 - FIFTH ITERATION received Friday, February 27, 2015 7:30 PM
previous commit mistakenly labeled SIXTH ITERATION
</commit_message>
<xml_diff>
--- a/etc/pm/requirements/Pre-K Finder and Form Modifications 2015 - Round 2.xlsx
+++ b/etc/pm/requirements/Pre-K Finder and Form Modifications 2015 - Round 2.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
-  <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25203"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24120" windowHeight="13620"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24120" windowHeight="13620" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Requirements" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Requirements!$A$1:$J$11</definedName>
   </definedNames>
-  <calcPr calcId="140001"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="122">
   <si>
     <t>Requirement</t>
   </si>
@@ -837,6 +837,9 @@
   </si>
   <si>
     <t>DoiTT to change from Search by "School" to Search by "Program"</t>
+  </si>
+  <si>
+    <t>x</t>
   </si>
 </sst>
 </file>
@@ -986,16 +989,16 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1026,15 +1029,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1075,9 +1069,6 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -1102,6 +1093,18 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="19">
@@ -1543,706 +1546,706 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J36"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="5" style="10" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.42578125" style="10" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="67.28515625" style="11" customWidth="1"/>
-    <col min="4" max="4" width="46.28515625" style="12" customWidth="1"/>
-    <col min="5" max="5" width="46.28515625" style="15" customWidth="1"/>
-    <col min="6" max="7" width="46.28515625" style="16" customWidth="1"/>
-    <col min="8" max="8" width="8.42578125" style="10" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.42578125" style="10" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="64.140625" style="10" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="8.85546875" style="9"/>
-    <col min="12" max="12" width="11.42578125" style="9" bestFit="1" customWidth="1"/>
-    <col min="13" max="16384" width="8.85546875" style="9"/>
+    <col min="1" max="1" width="5" style="7" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.5" style="7" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="67.33203125" style="8" customWidth="1"/>
+    <col min="4" max="4" width="46.33203125" style="9" customWidth="1"/>
+    <col min="5" max="5" width="46.33203125" style="12" customWidth="1"/>
+    <col min="6" max="7" width="46.33203125" style="13" customWidth="1"/>
+    <col min="8" max="8" width="8.5" style="7" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.5" style="7" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="64.1640625" style="7" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8.83203125" style="6"/>
+    <col min="12" max="12" width="11.5" style="6" bestFit="1" customWidth="1"/>
+    <col min="13" max="16384" width="8.83203125" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
+    <row r="1" spans="1:10">
+      <c r="A1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="E1" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="F1" s="8" t="s">
+      <c r="F1" s="5" t="s">
         <v>94</v>
       </c>
-      <c r="G1" s="8" t="s">
+      <c r="G1" s="5" t="s">
         <v>108</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="H1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="I1" s="5" t="s">
+      <c r="I1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="5" t="s">
+      <c r="J1" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="105" x14ac:dyDescent="0.25">
-      <c r="A2" s="10">
+    <row r="2" spans="1:10" ht="84">
+      <c r="A2" s="7">
         <v>1</v>
       </c>
-      <c r="B2" s="10" t="s">
+      <c r="B2" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="11" t="s">
+      <c r="C2" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="D2" s="12" t="s">
+      <c r="D2" s="9" t="s">
         <v>68</v>
       </c>
-      <c r="E2" s="13" t="s">
+      <c r="E2" s="10" t="s">
         <v>69</v>
       </c>
-      <c r="F2" s="14" t="s">
+      <c r="F2" s="11" t="s">
         <v>93</v>
       </c>
-      <c r="G2" s="14" t="s">
+      <c r="G2" s="11" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="60" x14ac:dyDescent="0.25">
-      <c r="A3" s="10">
+    <row r="3" spans="1:10" ht="42">
+      <c r="A3" s="7">
         <v>2</v>
       </c>
-      <c r="B3" s="10" t="s">
+      <c r="B3" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="11" t="s">
+      <c r="C3" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="F3" s="16" t="s">
+      <c r="F3" s="13" t="s">
         <v>95</v>
       </c>
-      <c r="G3" s="16" t="s">
+      <c r="G3" s="13" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="10">
+    <row r="4" spans="1:10">
+      <c r="A4" s="7">
         <v>3</v>
       </c>
-      <c r="B4" s="10" t="s">
+      <c r="B4" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="11" t="s">
+      <c r="C4" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="F4" s="16" t="s">
+      <c r="F4" s="13" t="s">
         <v>96</v>
       </c>
-      <c r="G4" s="16" t="s">
+      <c r="G4" s="13" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="75" x14ac:dyDescent="0.25">
-      <c r="A5" s="10">
+    <row r="5" spans="1:10" ht="56">
+      <c r="A5" s="7">
         <v>4</v>
       </c>
-      <c r="B5" s="10" t="s">
+      <c r="B5" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="11" t="s">
+      <c r="C5" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="D5" s="12" t="s">
+      <c r="D5" s="9" t="s">
         <v>63</v>
       </c>
-      <c r="E5" s="13" t="s">
+      <c r="E5" s="10" t="s">
         <v>70</v>
       </c>
-      <c r="F5" s="14" t="s">
+      <c r="F5" s="11" t="s">
         <v>95</v>
       </c>
-      <c r="G5" s="14" t="s">
+      <c r="G5" s="11" t="s">
         <v>81</v>
       </c>
-      <c r="I5" s="17"/>
-      <c r="J5" s="17"/>
-    </row>
-    <row r="6" spans="1:10" ht="45" x14ac:dyDescent="0.25">
-      <c r="A6" s="10">
+      <c r="I5" s="14"/>
+      <c r="J5" s="14"/>
+    </row>
+    <row r="6" spans="1:10" ht="42">
+      <c r="A6" s="7">
         <v>5</v>
       </c>
-      <c r="B6" s="10" t="s">
+      <c r="B6" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="C6" s="11" t="s">
+      <c r="C6" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="D6" s="12" t="s">
+      <c r="D6" s="9" t="s">
         <v>64</v>
       </c>
-      <c r="E6" s="15" t="s">
+      <c r="E6" s="12" t="s">
         <v>71</v>
       </c>
-      <c r="G6" s="16" t="s">
+      <c r="G6" s="13" t="s">
         <v>81</v>
       </c>
-      <c r="I6" s="17"/>
-      <c r="J6" s="18" t="s">
+      <c r="I6" s="14"/>
+      <c r="J6" s="15" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="75" x14ac:dyDescent="0.25">
-      <c r="A7" s="10">
+    <row r="7" spans="1:10" ht="56">
+      <c r="A7" s="7">
         <v>6</v>
       </c>
-      <c r="B7" s="10" t="s">
+      <c r="B7" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="11" t="s">
+      <c r="C7" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="D7" s="12" t="s">
+      <c r="D7" s="9" t="s">
         <v>65</v>
       </c>
-      <c r="E7" s="13" t="s">
+      <c r="E7" s="10" t="s">
         <v>72</v>
       </c>
-      <c r="F7" s="14" t="s">
+      <c r="F7" s="11" t="s">
         <v>97</v>
       </c>
-      <c r="G7" s="14" t="s">
+      <c r="G7" s="11" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="90" x14ac:dyDescent="0.25">
-      <c r="A8" s="10">
+    <row r="8" spans="1:10" ht="70">
+      <c r="A8" s="7">
         <v>7</v>
       </c>
-      <c r="B8" s="10" t="s">
+      <c r="B8" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="11" t="s">
+      <c r="C8" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="D8" s="12" t="s">
+      <c r="D8" s="9" t="s">
         <v>67</v>
       </c>
-      <c r="E8" s="15" t="s">
+      <c r="E8" s="12" t="s">
         <v>73</v>
       </c>
-      <c r="F8" s="16" t="s">
+      <c r="F8" s="13" t="s">
         <v>95</v>
       </c>
-      <c r="G8" s="16" t="s">
+      <c r="G8" s="13" t="s">
         <v>81</v>
       </c>
-      <c r="J8" s="19" t="s">
+      <c r="J8" s="25" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="75" x14ac:dyDescent="0.25">
-      <c r="A9" s="10">
+    <row r="9" spans="1:10" ht="56">
+      <c r="A9" s="7">
         <v>8</v>
       </c>
-      <c r="B9" s="10" t="s">
+      <c r="B9" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="C9" s="20" t="s">
+      <c r="C9" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="D9" s="12" t="s">
+      <c r="D9" s="9" t="s">
         <v>66</v>
       </c>
-      <c r="E9" s="13" t="s">
+      <c r="E9" s="10" t="s">
         <v>74</v>
       </c>
-      <c r="F9" s="14" t="s">
+      <c r="F9" s="11" t="s">
         <v>98</v>
       </c>
-      <c r="G9" s="14" t="s">
+      <c r="G9" s="11" t="s">
         <v>81</v>
       </c>
-      <c r="J9" s="19"/>
-    </row>
-    <row r="10" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A10" s="10">
+      <c r="J9" s="25"/>
+    </row>
+    <row r="10" spans="1:10">
+      <c r="A10" s="7">
         <v>9</v>
       </c>
-      <c r="B10" s="10" t="s">
+      <c r="B10" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="C10" s="20" t="s">
+      <c r="C10" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="F10" s="16" t="s">
+      <c r="F10" s="13" t="s">
         <v>95</v>
       </c>
-      <c r="G10" s="16" t="s">
+      <c r="G10" s="13" t="s">
         <v>81</v>
       </c>
-      <c r="J10" s="19"/>
-    </row>
-    <row r="11" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A11" s="10">
+      <c r="J10" s="25"/>
+    </row>
+    <row r="11" spans="1:10" ht="28">
+      <c r="A11" s="7">
         <v>10</v>
       </c>
-      <c r="B11" s="10" t="s">
+      <c r="B11" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="C11" s="11" t="s">
+      <c r="C11" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="F11" s="16" t="s">
+      <c r="F11" s="13" t="s">
         <v>95</v>
       </c>
-      <c r="G11" s="16" t="s">
+      <c r="G11" s="13" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="75" x14ac:dyDescent="0.25">
-      <c r="A12" s="10">
+    <row r="12" spans="1:10" ht="56">
+      <c r="A12" s="7">
         <v>11</v>
       </c>
-      <c r="B12" s="10" t="s">
+      <c r="B12" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="C12" s="11" t="s">
+      <c r="C12" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="F12" s="16" t="s">
+      <c r="F12" s="13" t="s">
         <v>95</v>
       </c>
-      <c r="G12" s="16" t="s">
+      <c r="G12" s="13" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="13" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A13" s="10">
+    <row r="13" spans="1:10" ht="28">
+      <c r="A13" s="7">
         <v>12</v>
       </c>
-      <c r="B13" s="10" t="s">
+      <c r="B13" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="C13" s="11" t="s">
+      <c r="C13" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="F13" s="16" t="s">
+      <c r="F13" s="13" t="s">
         <v>95</v>
       </c>
-      <c r="G13" s="16" t="s">
+      <c r="G13" s="13" t="s">
         <v>81</v>
       </c>
-      <c r="H13" s="9"/>
-      <c r="I13" s="9"/>
-      <c r="J13" s="9" t="s">
+      <c r="H13" s="6"/>
+      <c r="I13" s="6"/>
+      <c r="J13" s="6" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A14" s="10">
+    <row r="14" spans="1:10" ht="28">
+      <c r="A14" s="7">
         <v>13</v>
       </c>
-      <c r="B14" s="10" t="s">
+      <c r="B14" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="C14" s="11" t="s">
+      <c r="C14" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="D14" s="12" t="s">
+      <c r="D14" s="9" t="s">
         <v>56</v>
       </c>
-      <c r="E14" s="15" t="s">
+      <c r="E14" s="12" t="s">
         <v>75</v>
       </c>
-      <c r="F14" s="16" t="s">
+      <c r="F14" s="13" t="s">
         <v>95</v>
       </c>
-      <c r="G14" s="16" t="s">
+      <c r="G14" s="13" t="s">
         <v>81</v>
       </c>
-      <c r="H14" s="9"/>
-      <c r="I14" s="9"/>
-      <c r="J14" s="9"/>
-    </row>
-    <row r="15" spans="1:10" ht="75" x14ac:dyDescent="0.25">
-      <c r="A15" s="10">
+      <c r="H14" s="6"/>
+      <c r="I14" s="6"/>
+      <c r="J14" s="6"/>
+    </row>
+    <row r="15" spans="1:10" ht="56">
+      <c r="A15" s="7">
         <v>14</v>
       </c>
-      <c r="B15" s="10" t="s">
+      <c r="B15" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="C15" s="11" t="s">
+      <c r="C15" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="D15" s="12" t="s">
+      <c r="D15" s="9" t="s">
         <v>57</v>
       </c>
-      <c r="E15" s="13" t="s">
+      <c r="E15" s="10" t="s">
         <v>77</v>
       </c>
-      <c r="F15" s="14" t="s">
+      <c r="F15" s="11" t="s">
         <v>99</v>
       </c>
-      <c r="G15" s="14" t="s">
+      <c r="G15" s="11" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="16" spans="1:10" ht="75" x14ac:dyDescent="0.25">
-      <c r="A16" s="10">
+    <row r="16" spans="1:10" ht="70">
+      <c r="A16" s="7">
         <v>15</v>
       </c>
-      <c r="B16" s="10" t="s">
+      <c r="B16" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="C16" s="11" t="s">
+      <c r="C16" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="D16" s="12" t="s">
+      <c r="D16" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="E16" s="13" t="s">
+      <c r="E16" s="10" t="s">
         <v>76</v>
       </c>
-      <c r="F16" s="14" t="s">
+      <c r="F16" s="11" t="s">
         <v>100</v>
       </c>
-      <c r="G16" s="14" t="s">
+      <c r="G16" s="11" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="17" spans="1:10" s="27" customFormat="1" ht="90" x14ac:dyDescent="0.25">
-      <c r="A17" s="21">
+    <row r="17" spans="1:10" s="23" customFormat="1" ht="70">
+      <c r="A17" s="17">
         <v>16</v>
       </c>
-      <c r="B17" s="21" t="s">
+      <c r="B17" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="C17" s="22" t="s">
+      <c r="C17" s="18" t="s">
         <v>39</v>
       </c>
-      <c r="D17" s="23" t="s">
+      <c r="D17" s="19" t="s">
         <v>55</v>
       </c>
-      <c r="E17" s="24" t="s">
+      <c r="E17" s="20" t="s">
         <v>78</v>
       </c>
-      <c r="F17" s="25" t="s">
+      <c r="F17" s="21" t="s">
         <v>101</v>
       </c>
-      <c r="G17" s="25" t="s">
+      <c r="G17" s="21" t="s">
         <v>112</v>
       </c>
-      <c r="H17" s="21"/>
-      <c r="I17" s="21"/>
-      <c r="J17" s="26"/>
-    </row>
-    <row r="18" spans="1:10" ht="135" x14ac:dyDescent="0.25">
-      <c r="A18" s="10">
+      <c r="H17" s="17"/>
+      <c r="I17" s="17"/>
+      <c r="J17" s="22"/>
+    </row>
+    <row r="18" spans="1:10" ht="98">
+      <c r="A18" s="7">
         <v>17</v>
       </c>
-      <c r="B18" s="10" t="s">
+      <c r="B18" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="C18" s="11" t="s">
+      <c r="C18" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="D18" s="12" t="s">
+      <c r="D18" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="E18" s="13" t="s">
+      <c r="E18" s="10" t="s">
         <v>79</v>
       </c>
-      <c r="F18" s="14" t="s">
+      <c r="F18" s="11" t="s">
         <v>102</v>
       </c>
-      <c r="G18" s="14" t="s">
+      <c r="G18" s="11" t="s">
         <v>113</v>
       </c>
-      <c r="J18" s="28" t="s">
+      <c r="J18" s="24" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="19" spans="1:10" ht="45" x14ac:dyDescent="0.25">
-      <c r="A19" s="10">
+    <row r="19" spans="1:10" ht="28">
+      <c r="A19" s="7">
         <v>18</v>
       </c>
-      <c r="B19" s="10" t="s">
+      <c r="B19" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="C19" s="11" t="s">
+      <c r="C19" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="D19" s="12" t="s">
+      <c r="D19" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="E19" s="13" t="s">
+      <c r="E19" s="10" t="s">
         <v>80</v>
       </c>
-      <c r="F19" s="14" t="s">
+      <c r="F19" s="11" t="s">
         <v>103</v>
       </c>
-      <c r="G19" s="14" t="s">
+      <c r="G19" s="11" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="20" spans="1:10" ht="90" x14ac:dyDescent="0.25">
-      <c r="A20" s="10">
+    <row r="20" spans="1:10" ht="70">
+      <c r="A20" s="7">
         <v>19</v>
       </c>
-      <c r="B20" s="10" t="s">
+      <c r="B20" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="C20" s="11" t="s">
+      <c r="C20" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="D20" s="12" t="s">
+      <c r="D20" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="E20" s="15" t="s">
+      <c r="E20" s="12" t="s">
         <v>81</v>
       </c>
-      <c r="G20" s="16" t="s">
+      <c r="G20" s="13" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="21" spans="1:10" ht="75" x14ac:dyDescent="0.25">
-      <c r="A21" s="10">
+    <row r="21" spans="1:10" ht="56">
+      <c r="A21" s="7">
         <v>20</v>
       </c>
-      <c r="B21" s="10" t="s">
+      <c r="B21" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="C21" s="11" t="s">
+      <c r="C21" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="D21" s="12" t="s">
+      <c r="D21" s="9" t="s">
         <v>60</v>
       </c>
-      <c r="E21" s="15" t="s">
+      <c r="E21" s="12" t="s">
         <v>81</v>
       </c>
-      <c r="G21" s="16" t="s">
+      <c r="G21" s="13" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="22" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A22" s="10">
+    <row r="22" spans="1:10" ht="28">
+      <c r="A22" s="7">
         <v>21</v>
       </c>
-      <c r="B22" s="10" t="s">
+      <c r="B22" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="C22" s="11" t="s">
+      <c r="C22" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="G22" s="16" t="s">
+      <c r="G22" s="13" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="23" spans="1:10" ht="45" x14ac:dyDescent="0.25">
-      <c r="A23" s="10">
+    <row r="23" spans="1:10" ht="42">
+      <c r="A23" s="7">
         <v>22</v>
       </c>
-      <c r="B23" s="10" t="s">
+      <c r="B23" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="C23" s="11" t="s">
+      <c r="C23" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="D23" s="12" t="s">
+      <c r="D23" s="9" t="s">
         <v>61</v>
       </c>
-      <c r="E23" s="15" t="s">
+      <c r="E23" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="G23" s="16" t="s">
+      <c r="G23" s="13" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="24" spans="1:10" ht="60" x14ac:dyDescent="0.25">
-      <c r="A24" s="10">
+    <row r="24" spans="1:10" ht="56">
+      <c r="A24" s="7">
         <v>23</v>
       </c>
-      <c r="B24" s="10" t="s">
+      <c r="B24" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="C24" s="11" t="s">
+      <c r="C24" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="D24" s="12" t="s">
+      <c r="D24" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="E24" s="13" t="s">
+      <c r="E24" s="10" t="s">
         <v>83</v>
       </c>
-      <c r="F24" s="14" t="s">
+      <c r="F24" s="11" t="s">
         <v>104</v>
       </c>
-      <c r="G24" s="14" t="s">
+      <c r="G24" s="11" t="s">
         <v>116</v>
       </c>
-      <c r="J24" s="10" t="s">
+      <c r="J24" s="7" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="26" spans="1:10" ht="75" x14ac:dyDescent="0.25">
-      <c r="C26" s="7" t="s">
+    <row r="26" spans="1:10" ht="56">
+      <c r="C26" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="D26" s="12" t="s">
+      <c r="D26" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="E26" s="13" t="s">
+      <c r="E26" s="10" t="s">
         <v>84</v>
       </c>
-      <c r="F26" s="14" t="s">
+      <c r="F26" s="11" t="s">
         <v>105</v>
       </c>
-      <c r="G26" s="14"/>
-    </row>
-    <row r="28" spans="1:10" ht="60" x14ac:dyDescent="0.25">
-      <c r="A28" s="10">
+      <c r="G26" s="11"/>
+    </row>
+    <row r="28" spans="1:10" ht="42">
+      <c r="A28" s="7">
         <v>24</v>
       </c>
-      <c r="B28" s="10" t="s">
+      <c r="B28" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="C28" s="11" t="s">
+      <c r="C28" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="D28" s="12" t="s">
+      <c r="D28" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="F28" s="14" t="s">
+      <c r="F28" s="11" t="s">
         <v>99</v>
       </c>
-      <c r="G28" s="14" t="s">
+      <c r="G28" s="11" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="29" spans="1:10" ht="75" x14ac:dyDescent="0.25">
-      <c r="A29" s="10">
+    <row r="29" spans="1:10" ht="56">
+      <c r="A29" s="7">
         <v>25</v>
       </c>
-      <c r="B29" s="10" t="s">
+      <c r="B29" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="C29" s="11" t="s">
+      <c r="C29" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="D29" s="12" t="s">
+      <c r="D29" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="F29" s="14" t="s">
+      <c r="F29" s="11" t="s">
         <v>99</v>
       </c>
-      <c r="G29" s="14" t="s">
+      <c r="G29" s="11" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="30" spans="1:10" ht="105" x14ac:dyDescent="0.25">
-      <c r="A30" s="10">
+    <row r="30" spans="1:10" ht="84">
+      <c r="A30" s="7">
         <v>26</v>
       </c>
-      <c r="B30" s="10" t="s">
+      <c r="B30" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="C30" s="11" t="s">
+      <c r="C30" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="D30" s="12" t="s">
+      <c r="D30" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="E30" s="13" t="s">
+      <c r="E30" s="10" t="s">
         <v>86</v>
       </c>
-      <c r="F30" s="14" t="s">
+      <c r="F30" s="11" t="s">
         <v>106</v>
       </c>
-      <c r="G30" s="14" t="s">
+      <c r="G30" s="11" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="31" spans="1:10" s="27" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A31" s="21">
+    <row r="31" spans="1:10" s="23" customFormat="1" ht="42">
+      <c r="A31" s="17">
         <v>27</v>
       </c>
-      <c r="B31" s="21" t="s">
+      <c r="B31" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="C31" s="22" t="s">
+      <c r="C31" s="18" t="s">
         <v>44</v>
       </c>
-      <c r="D31" s="23" t="s">
+      <c r="D31" s="19" t="s">
         <v>50</v>
       </c>
-      <c r="E31" s="24"/>
-      <c r="F31" s="25"/>
-      <c r="G31" s="25" t="s">
+      <c r="E31" s="20"/>
+      <c r="F31" s="21"/>
+      <c r="G31" s="21" t="s">
         <v>81</v>
       </c>
-      <c r="H31" s="21"/>
-      <c r="I31" s="21"/>
-      <c r="J31" s="26"/>
-    </row>
-    <row r="32" spans="1:10" ht="120" x14ac:dyDescent="0.25">
-      <c r="A32" s="10">
+      <c r="H31" s="17"/>
+      <c r="I31" s="17"/>
+      <c r="J31" s="22"/>
+    </row>
+    <row r="32" spans="1:10" ht="98">
+      <c r="A32" s="7">
         <v>28</v>
       </c>
-      <c r="B32" s="10" t="s">
+      <c r="B32" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="C32" s="11" t="s">
+      <c r="C32" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="D32" s="12" t="s">
+      <c r="D32" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="E32" s="13" t="s">
+      <c r="E32" s="10" t="s">
         <v>85</v>
       </c>
-      <c r="F32" s="14" t="s">
+      <c r="F32" s="11" t="s">
         <v>107</v>
       </c>
-      <c r="G32" s="14" t="s">
+      <c r="G32" s="11" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="33" spans="1:10" ht="75" x14ac:dyDescent="0.25">
-      <c r="A33" s="10">
+    <row r="33" spans="1:10" ht="56">
+      <c r="A33" s="7">
         <v>29</v>
       </c>
-      <c r="B33" s="10" t="s">
+      <c r="B33" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="C33" s="11" t="s">
+      <c r="C33" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="D33" s="12" t="s">
+      <c r="D33" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="G33" s="16" t="s">
+      <c r="G33" s="13" t="s">
         <v>81</v>
       </c>
-      <c r="H33" s="9"/>
-      <c r="I33" s="9"/>
-      <c r="J33" s="9"/>
-    </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="H36" s="9"/>
-      <c r="I36" s="9"/>
-      <c r="J36" s="9"/>
+      <c r="H33" s="6"/>
+      <c r="I33" s="6"/>
+      <c r="J33" s="6"/>
+    </row>
+    <row r="36" spans="1:10">
+      <c r="H36" s="6"/>
+      <c r="I36" s="6"/>
+      <c r="J36" s="6"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:J11"/>
@@ -2250,8 +2253,8 @@
     <mergeCell ref="J8:J10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="3" orientation="landscape" r:id="rId1"/>
-  <legacyDrawing r:id="rId2"/>
+  <pageSetup paperSize="3" orientation="landscape"/>
+  <legacyDrawing r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -2262,18 +2265,18 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:D20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="2" max="2" width="30.85546875" customWidth="1"/>
+    <col min="2" max="2" width="30.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -2281,7 +2284,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -2289,12 +2292,17 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
         <v>4</v>
+      </c>
+    </row>
+    <row r="20" spans="4:4">
+      <c r="D20" t="s">
+        <v>121</v>
       </c>
     </row>
   </sheetData>
@@ -2315,60 +2323,60 @@
       <selection activeCell="B3" sqref="B3:F3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="5.85546875" customWidth="1"/>
-    <col min="7" max="7" width="5.85546875" customWidth="1"/>
-    <col min="13" max="13" width="5.85546875" customWidth="1"/>
+    <col min="1" max="1" width="5.83203125" customWidth="1"/>
+    <col min="7" max="7" width="5.83203125" customWidth="1"/>
+    <col min="13" max="13" width="5.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:18" ht="28.5" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B2" s="3" t="s">
+    <row r="2" spans="2:18" ht="28.5" customHeight="1">
+      <c r="B2" s="27" t="s">
         <v>88</v>
       </c>
-      <c r="C2" s="4"/>
-      <c r="D2" s="4"/>
-      <c r="E2" s="4"/>
-      <c r="F2" s="4"/>
-      <c r="H2" s="3" t="s">
+      <c r="C2" s="28"/>
+      <c r="D2" s="28"/>
+      <c r="E2" s="28"/>
+      <c r="F2" s="28"/>
+      <c r="H2" s="27" t="s">
         <v>89</v>
       </c>
-      <c r="I2" s="4"/>
-      <c r="J2" s="4"/>
-      <c r="K2" s="4"/>
-      <c r="L2" s="4"/>
-      <c r="N2" s="3" t="s">
+      <c r="I2" s="28"/>
+      <c r="J2" s="28"/>
+      <c r="K2" s="28"/>
+      <c r="L2" s="28"/>
+      <c r="N2" s="27" t="s">
         <v>89</v>
       </c>
-      <c r="O2" s="4"/>
-      <c r="P2" s="4"/>
-      <c r="Q2" s="4"/>
-      <c r="R2" s="4"/>
-    </row>
-    <row r="3" spans="2:18" ht="58.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="2" t="s">
+      <c r="O2" s="28"/>
+      <c r="P2" s="28"/>
+      <c r="Q2" s="28"/>
+      <c r="R2" s="28"/>
+    </row>
+    <row r="3" spans="2:18" ht="58.5" customHeight="1">
+      <c r="B3" s="26" t="s">
         <v>90</v>
       </c>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
+      <c r="C3" s="26"/>
+      <c r="D3" s="26"/>
+      <c r="E3" s="26"/>
+      <c r="F3" s="26"/>
       <c r="G3" s="1"/>
-      <c r="H3" s="2" t="s">
+      <c r="H3" s="26" t="s">
         <v>91</v>
       </c>
-      <c r="I3" s="2"/>
-      <c r="J3" s="2"/>
-      <c r="K3" s="2"/>
-      <c r="L3" s="2"/>
+      <c r="I3" s="26"/>
+      <c r="J3" s="26"/>
+      <c r="K3" s="26"/>
+      <c r="L3" s="26"/>
       <c r="M3" s="1"/>
-      <c r="N3" s="2" t="s">
+      <c r="N3" s="26" t="s">
         <v>92</v>
       </c>
-      <c r="O3" s="2"/>
-      <c r="P3" s="2"/>
-      <c r="Q3" s="2"/>
-      <c r="R3" s="2"/>
+      <c r="O3" s="26"/>
+      <c r="P3" s="26"/>
+      <c r="Q3" s="26"/>
+      <c r="R3" s="26"/>
     </row>
   </sheetData>
   <mergeCells count="6">
@@ -2380,7 +2388,12 @@
     <mergeCell ref="N3:R3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-  <drawing r:id="rId2"/>
+  <pageSetup orientation="portrait"/>
+  <drawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>